<commit_message>
fix per tracking file 20241112
</commit_message>
<xml_diff>
--- a/Integration Services Project2/notes/STR(DM-Transaction)-Appendix B - Test and PR Summary.xlsx
+++ b/Integration Services Project2/notes/STR(DM-Transaction)-Appendix B - Test and PR Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\STE.2022.CoswinMigration\Integration Services Project2\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{440BEF91-BD08-42F9-B3AE-8985F8807491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4282B71D-A5F3-4FE6-8492-8268A5260916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Summary" sheetId="6" r:id="rId1"/>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1515" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="410">
   <si>
     <t>Test Status</t>
   </si>
@@ -900,20 +900,6 @@
     <t>A new field to be created. CONTRACT.STE_REMARKS</t>
   </si>
   <si>
-    <t>Map ITEM_INFO via ITEM_ instead of directly from STOREITEM.
-Please verify the following fields:
-MAXLEVEL
-MINLEVEL
-SSTOCK
-DELIVERYTIME
-ISSUE1YRAGO
-ISSUE2YRAGO
-CURBALTOTAL
-AVBLBALANCE
-RESERVEDQTY
-ORDERQTY</t>
-  </si>
-  <si>
     <t>Map to new fields: STE_CSWNSUPPLIER</t>
   </si>
   <si>
@@ -957,16 +943,6 @@
 WHEN DEM_STATUS=51 THEN 'CAN'
 WHEN DEM_STATUS=52 THEN 'WAPPR'
 WHEN DEM_STATUS=57 THEN 'APPR'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Material Requisions status mapping:
-4.
-   48 - 0 - No Issued - APPR
-   49 - 1 - Part Issued  - APPR
-   50 - 2 - Issue Completed - CLOSE
-   51 - 3 - Cancelled -  CAN
-   52 - 4 - Not Validated - WAPPR
-   57 - 9- Directly Issued - CLOSE </t>
   </si>
   <si>
     <t xml:space="preserve">Default the properties as standard values based on when contract type is selected as “BLANKET”,”PRICE” using scripts.
@@ -1587,6 +1563,15 @@
   </si>
   <si>
     <t>New calculated field</t>
+  </si>
+  <si>
+    <t>CHARTOFACCOUNTS</t>
+  </si>
+  <si>
+    <t>New custom column: CHARTOFACCOUNTS.STE_MIGRATIONSOURCE</t>
+  </si>
+  <si>
+    <t>New custom column: MATRECTRANS.STE_MIGRATIONSOURCE</t>
   </si>
 </sst>
 </file>
@@ -1883,7 +1868,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2070,6 +2055,12 @@
     <xf numFmtId="49" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2085,17 +2076,10 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3047,18 +3031,18 @@
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="C3" s="70" t="s">
+      <c r="C3" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="72" t="s">
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="73"/>
-      <c r="I3" s="73"/>
-      <c r="J3" s="74"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="75"/>
+      <c r="J3" s="76"/>
       <c r="K3" s="3" t="s">
         <v>61</v>
       </c>
@@ -3879,8 +3863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView topLeftCell="H73" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="N75" sqref="N75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3952,13 +3936,13 @@
       </c>
       <c r="N1" s="30"/>
       <c r="O1" s="58" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="P1" s="30" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="Q1" s="30" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="R1" s="30" t="s">
         <v>53</v>
@@ -4005,22 +3989,22 @@
       </c>
       <c r="K2" s="36"/>
       <c r="L2" s="34" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="M2" s="34" t="s">
         <v>230</v>
       </c>
       <c r="N2" s="34" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O2" s="59" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="P2" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="Q2" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R2" s="34"/>
       <c r="S2" s="36"/>
@@ -4050,20 +4034,20 @@
       </c>
       <c r="K3" s="36"/>
       <c r="L3" s="34" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="M3" s="34" t="s">
         <v>231</v>
       </c>
       <c r="N3" s="34" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="O3" s="59"/>
       <c r="P3" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="Q3" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R3" s="34"/>
       <c r="S3" s="36"/>
@@ -4099,14 +4083,14 @@
         <v>133</v>
       </c>
       <c r="N4" s="34" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="O4" s="59"/>
       <c r="P4" s="34" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="Q4" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R4" s="34"/>
       <c r="S4" s="36"/>
@@ -4142,16 +4126,16 @@
         <v>232</v>
       </c>
       <c r="N5" s="34" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="O5" s="59">
         <v>309</v>
       </c>
       <c r="P5" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="Q5" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R5" s="34"/>
       <c r="S5" s="36"/>
@@ -4189,14 +4173,14 @@
         <v>232</v>
       </c>
       <c r="N6" s="34" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="O6" s="59"/>
       <c r="P6" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="Q6" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R6" s="34"/>
       <c r="S6" s="36"/>
@@ -4234,16 +4218,16 @@
         <v>135</v>
       </c>
       <c r="N7" s="34" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="O7" s="59" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="P7" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="Q7" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R7" s="34"/>
       <c r="S7" s="36"/>
@@ -4279,16 +4263,16 @@
         <v>136</v>
       </c>
       <c r="N8" s="34" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="O8" s="59" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="P8" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="Q8" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R8" s="34"/>
       <c r="S8" s="36"/>
@@ -4327,13 +4311,13 @@
         <v>236</v>
       </c>
       <c r="O9" s="59" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="P9" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="Q9" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R9" s="34"/>
       <c r="S9" s="36"/>
@@ -4369,14 +4353,14 @@
         <v>165</v>
       </c>
       <c r="N10" s="49" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="O10" s="69"/>
       <c r="P10" s="49" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="Q10" s="49" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="R10" s="45"/>
       <c r="S10" s="44"/>
@@ -4412,16 +4396,16 @@
         <v>139</v>
       </c>
       <c r="N11" s="34" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="O11" s="59" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="P11" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="Q11" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R11" s="34"/>
       <c r="S11" s="36"/>
@@ -4457,16 +4441,16 @@
         <v>140</v>
       </c>
       <c r="N12" s="34" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="O12" s="59" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="P12" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="Q12" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R12" s="34"/>
       <c r="S12" s="36"/>
@@ -4489,7 +4473,7 @@
         <v>65</v>
       </c>
       <c r="I13" s="48" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="J13" s="33" t="s">
         <v>121</v>
@@ -4501,17 +4485,17 @@
       <c r="M13" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="N13" s="75" t="s">
-        <v>289</v>
+      <c r="N13" s="34" t="s">
+        <v>287</v>
       </c>
       <c r="O13" s="59" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="P13" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="Q13" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R13" s="34"/>
       <c r="S13" s="36"/>
@@ -4547,14 +4531,14 @@
         <v>142</v>
       </c>
       <c r="N14" s="34" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="O14" s="59"/>
       <c r="P14" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="Q14" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R14" s="34"/>
       <c r="S14" s="36"/>
@@ -4592,14 +4576,14 @@
         <v>142</v>
       </c>
       <c r="N15" s="34" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="O15" s="59"/>
       <c r="P15" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="Q15" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R15" s="34"/>
       <c r="S15" s="36"/>
@@ -4637,14 +4621,14 @@
         <v>138</v>
       </c>
       <c r="N16" s="49" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="O16" s="59"/>
       <c r="P16" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="Q16" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R16" s="34"/>
       <c r="S16" s="36"/>
@@ -4680,14 +4664,14 @@
         <v>144</v>
       </c>
       <c r="N17" s="34" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="O17" s="59"/>
       <c r="P17" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="Q17" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R17" s="34"/>
       <c r="S17" s="36"/>
@@ -4723,14 +4707,14 @@
         <v>145</v>
       </c>
       <c r="N18" s="32" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="O18" s="60"/>
       <c r="P18" s="32" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="Q18" s="32" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R18" s="45"/>
       <c r="S18" s="44"/>
@@ -4766,16 +4750,16 @@
         <v>142</v>
       </c>
       <c r="N19" s="34" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="O19" s="59" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="P19" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="Q19" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R19" s="45"/>
       <c r="S19" s="44"/>
@@ -4813,14 +4797,14 @@
         <v>146</v>
       </c>
       <c r="N20" s="34" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="O20" s="59"/>
       <c r="P20" s="34" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="Q20" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R20" s="45"/>
       <c r="S20" s="44"/>
@@ -4858,14 +4842,14 @@
         <v>143</v>
       </c>
       <c r="N21" s="49" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="O21" s="59"/>
       <c r="P21" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="Q21" s="50" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="R21" s="34"/>
       <c r="S21" s="36"/>
@@ -4903,10 +4887,10 @@
       <c r="N22" s="34"/>
       <c r="O22" s="59"/>
       <c r="P22" s="34" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="Q22" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R22" s="45"/>
       <c r="S22" s="44"/>
@@ -4942,14 +4926,14 @@
         <v>149</v>
       </c>
       <c r="N23" s="34" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="O23" s="59"/>
       <c r="P23" s="34" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="Q23" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R23" s="45"/>
       <c r="S23" s="44"/>
@@ -4985,14 +4969,14 @@
         <v>151</v>
       </c>
       <c r="N24" s="34" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="O24" s="59"/>
       <c r="P24" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="Q24" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R24" s="45"/>
       <c r="S24" s="44"/>
@@ -5028,14 +5012,14 @@
         <v>153</v>
       </c>
       <c r="N25" s="34" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="O25" s="68"/>
-      <c r="P25" s="75" t="s">
-        <v>296</v>
-      </c>
-      <c r="Q25" s="75" t="s">
-        <v>284</v>
+      <c r="P25" s="34" t="s">
+        <v>294</v>
+      </c>
+      <c r="Q25" s="34" t="s">
+        <v>282</v>
       </c>
       <c r="R25" s="45"/>
       <c r="S25" s="44"/>
@@ -5073,14 +5057,14 @@
         <v>159</v>
       </c>
       <c r="N26" s="34" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="O26" s="59"/>
       <c r="P26" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="Q26" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R26" s="45"/>
       <c r="S26" s="44"/>
@@ -5120,10 +5104,10 @@
       </c>
       <c r="O27" s="59"/>
       <c r="P27" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="Q27" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R27" s="45"/>
       <c r="S27" s="44"/>
@@ -5159,14 +5143,14 @@
         <v>161</v>
       </c>
       <c r="N28" s="34" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="O28" s="59"/>
       <c r="P28" s="34" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="Q28" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R28" s="45"/>
       <c r="S28" s="44"/>
@@ -5204,14 +5188,14 @@
         <v>147</v>
       </c>
       <c r="N29" s="49" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="O29" s="59"/>
       <c r="P29" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="Q29" s="50" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="R29" s="45"/>
       <c r="S29" s="44"/>
@@ -5247,14 +5231,14 @@
         <v>232</v>
       </c>
       <c r="N30" s="34" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="O30" s="59"/>
       <c r="P30" s="34" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="Q30" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R30" s="45"/>
       <c r="S30" s="44"/>
@@ -5290,14 +5274,14 @@
         <v>162</v>
       </c>
       <c r="N31" s="49" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="O31" s="59"/>
       <c r="P31" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="Q31" s="50" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="R31" s="45"/>
       <c r="S31" s="44"/>
@@ -5337,10 +5321,10 @@
       </c>
       <c r="O32" s="59"/>
       <c r="P32" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="Q32" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R32" s="45"/>
       <c r="S32" s="44"/>
@@ -5370,20 +5354,20 @@
       </c>
       <c r="K33" s="34"/>
       <c r="L33" s="34" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="M33" s="34" t="s">
         <v>162</v>
       </c>
       <c r="N33" s="34" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="O33" s="59"/>
       <c r="P33" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="Q33" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R33" s="45"/>
       <c r="S33" s="44"/>
@@ -5413,20 +5397,20 @@
       </c>
       <c r="K34" s="34"/>
       <c r="L34" s="34" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="M34" s="34" t="s">
         <v>162</v>
       </c>
       <c r="N34" s="34" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="O34" s="59"/>
       <c r="P34" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="Q34" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R34" s="45"/>
       <c r="S34" s="44"/>
@@ -5462,14 +5446,14 @@
         <v>165</v>
       </c>
       <c r="N35" s="34" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="O35" s="59"/>
       <c r="P35" s="34" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="Q35" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R35" s="45"/>
       <c r="S35" s="44"/>
@@ -5505,14 +5489,14 @@
         <v>170</v>
       </c>
       <c r="N36" s="34" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="O36" s="59"/>
       <c r="P36" s="34" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="Q36" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R36" s="45"/>
       <c r="S36" s="44"/>
@@ -5548,14 +5532,14 @@
         <v>170</v>
       </c>
       <c r="N37" s="34" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="O37" s="59"/>
       <c r="P37" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="Q37" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R37" s="45"/>
       <c r="S37" s="44"/>
@@ -5595,10 +5579,10 @@
       </c>
       <c r="O38" s="59"/>
       <c r="P38" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="Q38" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R38" s="45"/>
       <c r="S38" s="44"/>
@@ -5636,10 +5620,10 @@
       <c r="N39" s="34"/>
       <c r="O39" s="59"/>
       <c r="P39" s="34" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="Q39" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R39" s="45"/>
       <c r="S39" s="44"/>
@@ -5679,10 +5663,10 @@
       </c>
       <c r="O40" s="59"/>
       <c r="P40" s="34" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="Q40" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R40" s="45"/>
       <c r="S40" s="44"/>
@@ -5724,10 +5708,10 @@
       </c>
       <c r="O41" s="59"/>
       <c r="P41" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="Q41" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R41" s="45"/>
       <c r="S41" s="44"/>
@@ -5763,14 +5747,14 @@
         <v>211</v>
       </c>
       <c r="N42" s="49" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="O42" s="59"/>
       <c r="P42" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="Q42" s="50" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="R42" s="45"/>
       <c r="S42" s="44"/>
@@ -5806,14 +5790,14 @@
         <v>211</v>
       </c>
       <c r="N43" s="34" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="O43" s="59"/>
       <c r="P43" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="Q43" s="50" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="R43" s="45"/>
       <c r="S43" s="44"/>
@@ -5855,10 +5839,10 @@
       </c>
       <c r="O44" s="59"/>
       <c r="P44" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="Q44" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R44" s="45"/>
       <c r="S44" s="44"/>
@@ -5896,10 +5880,10 @@
       <c r="N45" s="34"/>
       <c r="O45" s="59"/>
       <c r="P45" s="34" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q45" s="34" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="R45" s="45"/>
       <c r="S45" s="44"/>
@@ -5937,10 +5921,10 @@
       <c r="N46" s="34"/>
       <c r="O46" s="59"/>
       <c r="P46" s="34" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q46" s="34" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="R46" s="45"/>
       <c r="S46" s="44"/>
@@ -5965,7 +5949,7 @@
         <v>79</v>
       </c>
       <c r="I47" s="34" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="J47" s="33" t="s">
         <v>121</v>
@@ -5980,10 +5964,10 @@
       <c r="N47" s="34"/>
       <c r="O47" s="59"/>
       <c r="P47" s="34" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q47" s="34" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="R47" s="45"/>
       <c r="S47" s="44"/>
@@ -6023,10 +6007,10 @@
       <c r="N48" s="34"/>
       <c r="O48" s="59"/>
       <c r="P48" s="34" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q48" s="34" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="R48" s="45"/>
       <c r="S48" s="44"/>
@@ -6064,10 +6048,10 @@
       <c r="N49" s="34"/>
       <c r="O49" s="59"/>
       <c r="P49" s="34" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q49" s="34" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="R49" s="45"/>
       <c r="S49" s="44"/>
@@ -6107,10 +6091,10 @@
       <c r="N50" s="34"/>
       <c r="O50" s="59"/>
       <c r="P50" s="34" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q50" s="34" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="R50" s="45"/>
       <c r="S50" s="44"/>
@@ -6150,10 +6134,10 @@
       <c r="N51" s="34"/>
       <c r="O51" s="59"/>
       <c r="P51" s="34" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q51" s="34" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="R51" s="45"/>
       <c r="S51" s="44"/>
@@ -6191,10 +6175,10 @@
       <c r="N52" s="34"/>
       <c r="O52" s="59"/>
       <c r="P52" s="34" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q52" s="34" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="R52" s="45"/>
       <c r="S52" s="44"/>
@@ -6234,10 +6218,10 @@
       <c r="N53" s="34"/>
       <c r="O53" s="59"/>
       <c r="P53" s="34" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q53" s="34" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="R53" s="45"/>
       <c r="S53" s="44"/>
@@ -6275,10 +6259,10 @@
       <c r="N54" s="34"/>
       <c r="O54" s="59"/>
       <c r="P54" s="34" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q54" s="34" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="R54" s="45"/>
       <c r="S54" s="44"/>
@@ -6318,10 +6302,10 @@
       <c r="N55" s="34"/>
       <c r="O55" s="59"/>
       <c r="P55" s="34" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q55" s="34" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="R55" s="45"/>
       <c r="S55" s="44"/>
@@ -6361,10 +6345,10 @@
       <c r="N56" s="34"/>
       <c r="O56" s="59"/>
       <c r="P56" s="34" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q56" s="34" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="R56" s="45"/>
       <c r="S56" s="44"/>
@@ -6404,10 +6388,10 @@
       <c r="N57" s="34"/>
       <c r="O57" s="59"/>
       <c r="P57" s="34" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q57" s="34" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="R57" s="45"/>
       <c r="S57" s="44"/>
@@ -6445,10 +6429,10 @@
       <c r="N58" s="34"/>
       <c r="O58" s="59"/>
       <c r="P58" s="34" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q58" s="34" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="R58" s="45"/>
       <c r="S58" s="44"/>
@@ -6484,14 +6468,14 @@
         <v>211</v>
       </c>
       <c r="N59" s="34" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="O59" s="59"/>
       <c r="P59" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="Q59" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R59" s="45"/>
       <c r="S59" s="44"/>
@@ -6513,7 +6497,7 @@
       <c r="H60" s="35" t="s">
         <v>191</v>
       </c>
-      <c r="I60" s="77" t="s">
+      <c r="I60" s="70" t="s">
         <v>193</v>
       </c>
       <c r="J60" s="33" t="s">
@@ -6527,14 +6511,14 @@
         <v>221</v>
       </c>
       <c r="N60" s="34" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="O60" s="59"/>
       <c r="P60" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="Q60" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R60" s="45"/>
       <c r="S60" s="44"/>
@@ -6570,14 +6554,14 @@
         <v>211</v>
       </c>
       <c r="N61" s="34" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="O61" s="59"/>
       <c r="P61" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="Q61" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R61" s="45"/>
       <c r="S61" s="44"/>
@@ -6607,20 +6591,20 @@
       </c>
       <c r="K62" s="34"/>
       <c r="L62" s="34" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="M62" s="34" t="s">
         <v>211</v>
       </c>
       <c r="N62" s="34" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="O62" s="59"/>
       <c r="P62" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="Q62" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R62" s="45"/>
       <c r="S62" s="44"/>
@@ -6656,14 +6640,14 @@
         <v>211</v>
       </c>
       <c r="N63" s="34" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="O63" s="59"/>
       <c r="P63" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="Q63" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R63" s="45"/>
       <c r="S63" s="44"/>
@@ -6701,14 +6685,14 @@
         <v>211</v>
       </c>
       <c r="N64" s="34" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="O64" s="59"/>
       <c r="P64" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="Q64" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R64" s="45"/>
       <c r="S64" s="44"/>
@@ -6746,14 +6730,14 @@
         <v>211</v>
       </c>
       <c r="N65" s="34" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="O65" s="59"/>
       <c r="P65" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="Q65" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R65" s="45"/>
       <c r="S65" s="44"/>
@@ -6785,20 +6769,20 @@
       </c>
       <c r="K66" s="34"/>
       <c r="L66" s="34" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="M66" s="34" t="s">
         <v>211</v>
       </c>
       <c r="N66" s="49" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="O66" s="59"/>
       <c r="P66" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="Q66" s="50" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="R66" s="45"/>
       <c r="S66" s="44"/>
@@ -6836,14 +6820,14 @@
         <v>211</v>
       </c>
       <c r="N67" s="63" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="O67" s="55"/>
       <c r="P67" s="34" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="Q67" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R67" s="45"/>
       <c r="S67" s="44"/>
@@ -6879,14 +6863,14 @@
         <v>211</v>
       </c>
       <c r="N68" s="34" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="O68" s="59"/>
       <c r="P68" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="Q68" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R68" s="45"/>
       <c r="S68" s="44"/>
@@ -6922,14 +6906,14 @@
         <v>211</v>
       </c>
       <c r="N69" s="34" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="O69" s="59"/>
       <c r="P69" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="Q69" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R69" s="45"/>
       <c r="S69" s="44"/>
@@ -6949,7 +6933,7 @@
       <c r="F70" s="44"/>
       <c r="G70" s="44"/>
       <c r="H70" s="35" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I70" s="48" t="s">
         <v>204</v>
@@ -6959,20 +6943,20 @@
       </c>
       <c r="K70" s="34"/>
       <c r="L70" s="34" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="M70" s="34" t="s">
         <v>211</v>
       </c>
       <c r="N70" s="34" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="O70" s="59"/>
       <c r="P70" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="Q70" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R70" s="45"/>
       <c r="S70" s="44"/>
@@ -6992,7 +6976,7 @@
       <c r="F71" s="44"/>
       <c r="G71" s="44"/>
       <c r="H71" s="35" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I71" s="48" t="s">
         <v>205</v>
@@ -7008,14 +6992,14 @@
         <v>211</v>
       </c>
       <c r="N71" s="34" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="O71" s="59"/>
       <c r="P71" s="34" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="Q71" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R71" s="45"/>
       <c r="S71" s="44"/>
@@ -7035,7 +7019,7 @@
       <c r="F72" s="44"/>
       <c r="G72" s="44"/>
       <c r="H72" s="35" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I72" s="48" t="s">
         <v>206</v>
@@ -7045,20 +7029,20 @@
       </c>
       <c r="K72" s="34"/>
       <c r="L72" s="34" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="M72" s="34" t="s">
         <v>211</v>
       </c>
       <c r="N72" s="49" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="O72" s="59"/>
       <c r="P72" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="Q72" s="50" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="R72" s="45"/>
       <c r="S72" s="44"/>
@@ -7078,16 +7062,16 @@
       <c r="F73" s="44"/>
       <c r="G73" s="44"/>
       <c r="H73" s="35" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I73" s="48" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="J73" s="33" t="s">
         <v>121</v>
       </c>
       <c r="K73" s="34" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="L73" s="34" t="s">
         <v>211</v>
@@ -7096,14 +7080,14 @@
         <v>211</v>
       </c>
       <c r="N73" s="34" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="O73" s="59"/>
       <c r="P73" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="Q73" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R73" s="45"/>
       <c r="S73" s="44"/>
@@ -7123,7 +7107,7 @@
       <c r="F74" s="44"/>
       <c r="G74" s="44"/>
       <c r="H74" s="35" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I74" s="48" t="s">
         <v>207</v>
@@ -7139,14 +7123,14 @@
         <v>211</v>
       </c>
       <c r="N74" s="34" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="O74" s="59"/>
       <c r="P74" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="Q74" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R74" s="45"/>
       <c r="S74" s="44"/>
@@ -7166,9 +7150,9 @@
       <c r="F75" s="44"/>
       <c r="G75" s="44"/>
       <c r="H75" s="35" t="s">
-        <v>247</v>
-      </c>
-      <c r="I75" s="78" t="s">
+        <v>246</v>
+      </c>
+      <c r="I75" s="71" t="s">
         <v>208</v>
       </c>
       <c r="J75" s="33" t="s">
@@ -7182,14 +7166,14 @@
         <v>211</v>
       </c>
       <c r="N75" s="49" t="s">
-        <v>393</v>
-      </c>
-      <c r="O75" s="76"/>
+        <v>391</v>
+      </c>
+      <c r="O75" s="59"/>
       <c r="P75" s="49" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="Q75" s="50" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="R75" s="45"/>
       <c r="S75" s="44"/>
@@ -7209,7 +7193,7 @@
       <c r="F76" s="44"/>
       <c r="G76" s="44"/>
       <c r="H76" s="35" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I76" s="48" t="s">
         <v>209</v>
@@ -7219,20 +7203,20 @@
       </c>
       <c r="K76" s="34"/>
       <c r="L76" s="34" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="M76" s="34" t="s">
         <v>211</v>
       </c>
       <c r="N76" s="34" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="O76" s="59"/>
       <c r="P76" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="Q76" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R76" s="45"/>
       <c r="S76" s="44"/>
@@ -7252,7 +7236,7 @@
       <c r="F77" s="44"/>
       <c r="G77" s="44"/>
       <c r="H77" s="35" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I77" s="48" t="s">
         <v>210</v>
@@ -7268,16 +7252,16 @@
         <v>211</v>
       </c>
       <c r="N77" s="34" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="O77" s="59">
         <v>206</v>
       </c>
       <c r="P77" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="Q77" s="50" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="R77" s="45"/>
       <c r="S77" s="44"/>
@@ -10049,10 +10033,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB88DB5-3756-408C-974A-7C21E554649F}">
-  <dimension ref="A1:J63"/>
+  <dimension ref="A1:J68"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48:F48"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -10066,24 +10050,24 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="56" t="s">
+        <v>251</v>
+      </c>
+      <c r="B1" t="s">
         <v>252</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>253</v>
       </c>
-      <c r="C1" t="s">
-        <v>254</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D2" s="2" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F2" s="2">
         <v>20</v>
@@ -10091,32 +10075,32 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="56" t="s">
+        <v>254</v>
+      </c>
+      <c r="B4" t="s">
         <v>255</v>
       </c>
-      <c r="B4" t="s">
-        <v>256</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="G4" s="57" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D5" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G5" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D6" s="2" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F6" s="2">
         <v>20</v>
@@ -10124,10 +10108,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D7" s="2" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F7" s="2">
         <v>20</v>
@@ -10135,10 +10119,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D8" s="2" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F8" s="2">
         <v>16</v>
@@ -10146,10 +10130,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D9" s="2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F9" s="2">
         <v>12</v>
@@ -10157,82 +10141,82 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D10" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F10" s="2">
         <v>32000</v>
       </c>
       <c r="G10" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="56" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B12" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D13" s="2" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F13" s="2">
         <v>32000</v>
       </c>
       <c r="G13" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A15" s="56" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B15" t="s">
+        <v>271</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>273</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D16" s="2" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D17" s="2" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F17" s="2">
         <v>32000</v>
       </c>
       <c r="G17" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
       <c r="D18" s="19" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E18" s="64" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F18" s="55">
         <v>16</v>
@@ -10240,54 +10224,54 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="56" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B20" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D21" s="2" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D22" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="G22" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D23" s="2" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F23" s="2">
         <v>32000</v>
       </c>
       <c r="G23" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D24" s="2" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F24" s="2">
         <v>110</v>
@@ -10295,16 +10279,16 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="56" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B26" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F26" s="2">
         <v>12</v>
@@ -10312,16 +10296,16 @@
     </row>
     <row r="28" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A28" s="56" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B28" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E28" s="64" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F28" s="55">
         <v>16</v>
@@ -10331,10 +10315,10 @@
     </row>
     <row r="29" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
       <c r="D29" s="64" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="E29" s="64" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F29" s="55">
         <v>10</v>
@@ -10344,42 +10328,42 @@
     </row>
     <row r="30" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
       <c r="D30" s="64" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E30" s="64" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F30" s="55" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="G30" s="64"/>
       <c r="H30" s="55"/>
     </row>
     <row r="31" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
       <c r="D31" s="64" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E31" s="64" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F31" s="55" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="G31" s="64"/>
       <c r="H31" s="55"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="56" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B33" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D33" s="19" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="E33" s="65" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F33" s="32">
         <v>16</v>
@@ -10391,10 +10375,10 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D34" s="19" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E34" s="19" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F34" s="66">
         <v>20</v>
@@ -10406,10 +10390,10 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D35" s="19" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E35" s="65" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="F35" s="32">
         <v>10</v>
@@ -10421,10 +10405,10 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E36" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F36" s="67">
         <v>15</v>
@@ -10433,10 +10417,10 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D37" s="19" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="E37" s="65" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="F37" s="32">
         <v>10</v>
@@ -10448,10 +10432,10 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D38" s="19" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E38" s="65" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F38" s="32">
         <v>10</v>
@@ -10463,10 +10447,10 @@
     </row>
     <row r="39" spans="1:10" ht="14.4" x14ac:dyDescent="0.25">
       <c r="D39" s="64" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="E39" s="64" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F39" s="64">
         <v>10</v>
@@ -10478,10 +10462,10 @@
     </row>
     <row r="40" spans="1:10" ht="14.4" x14ac:dyDescent="0.25">
       <c r="D40" s="64" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="E40" s="64" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F40" s="64">
         <v>20</v>
@@ -10493,10 +10477,10 @@
     </row>
     <row r="41" spans="1:10" ht="14.4" x14ac:dyDescent="0.25">
       <c r="D41" s="64" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E41" s="64" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="F41" s="64">
         <v>10</v>
@@ -10508,10 +10492,10 @@
     </row>
     <row r="42" spans="1:10" ht="14.4" x14ac:dyDescent="0.25">
       <c r="D42" s="64" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="E42" s="64" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F42" s="64">
         <v>10</v>
@@ -10523,10 +10507,10 @@
     </row>
     <row r="43" spans="1:10" ht="14.4" x14ac:dyDescent="0.25">
       <c r="D43" s="64" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E43" s="64" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="F43" s="64">
         <v>3</v>
@@ -10538,10 +10522,10 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D44" s="19" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E44" s="65" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="F44" s="32">
         <v>3</v>
@@ -10553,10 +10537,10 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E45" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="F45" s="67">
         <v>10</v>
@@ -10565,10 +10549,10 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D46" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E46" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F46" s="67">
         <v>15</v>
@@ -10577,10 +10561,10 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D47" s="19" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E47" s="65" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="F47" s="32">
         <v>3</v>
@@ -10592,131 +10576,175 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D48" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F48" s="2">
         <v>32000</v>
       </c>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F50" s="2">
         <v>20</v>
       </c>
     </row>
-    <row r="52" spans="2:6" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
+        <v>366</v>
+      </c>
+      <c r="D52" s="64" t="s">
         <v>368</v>
       </c>
-      <c r="D52" s="64" t="s">
+      <c r="E52" s="64" t="s">
+        <v>319</v>
+      </c>
+      <c r="F52" s="55" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="D53" s="64" t="s">
+        <v>369</v>
+      </c>
+      <c r="E53" s="64" t="s">
+        <v>319</v>
+      </c>
+      <c r="F53" s="55" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="D54" s="64" t="s">
         <v>370</v>
       </c>
-      <c r="E52" s="64" t="s">
-        <v>321</v>
-      </c>
-      <c r="F52" s="55" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="53" spans="2:6" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="D53" s="64" t="s">
+      <c r="E54" s="64" t="s">
+        <v>319</v>
+      </c>
+      <c r="F54" s="55" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="D55" s="64" t="s">
         <v>371</v>
       </c>
-      <c r="E53" s="64" t="s">
-        <v>321</v>
-      </c>
-      <c r="F53" s="55" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="54" spans="2:6" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="D54" s="64" t="s">
-        <v>372</v>
-      </c>
-      <c r="E54" s="64" t="s">
-        <v>321</v>
-      </c>
-      <c r="F54" s="55" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="55" spans="2:6" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="D55" s="64" t="s">
-        <v>373</v>
-      </c>
       <c r="E55" s="64" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F55" s="55">
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="2:6" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
       <c r="D56" s="64" t="s">
+        <v>379</v>
+      </c>
+      <c r="E56" s="64" t="s">
+        <v>319</v>
+      </c>
+      <c r="F56" s="55" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
         <v>381</v>
       </c>
-      <c r="E56" s="64" t="s">
-        <v>321</v>
-      </c>
-      <c r="F56" s="55" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
-        <v>383</v>
-      </c>
       <c r="D58" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="F58" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D60" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F60" s="2">
         <v>32000</v>
       </c>
     </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D62" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F62" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D63"/>
+    <row r="63" spans="1:6" s="78" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="77"/>
+      <c r="E63" s="79"/>
+      <c r="F63" s="79"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>407</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="F64" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>323</v>
+      </c>
+      <c r="D66" t="s">
+        <v>392</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="F66" s="2">
+        <v>32000</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>383</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="F68" s="2">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- Merged Gareth' pkg (not tested)
</commit_message>
<xml_diff>
--- a/Integration Services Project2/notes/STR(DM-Transaction)-Appendix B - Test and PR Summary.xlsx
+++ b/Integration Services Project2/notes/STR(DM-Transaction)-Appendix B - Test and PR Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\STE.2022.CoswinMigration\Integration Services Project2\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFAC31D9-F69A-4331-A587-B55322DEDC46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{770F6342-63FB-4660-9B41-97C4B4272B16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="417">
   <si>
     <t>Test Status</t>
   </si>
@@ -1582,6 +1582,18 @@
   </si>
   <si>
     <t>Need to extend POLINE.GLDEBITACCT to 110 char</t>
+  </si>
+  <si>
+    <t>PERSON</t>
+  </si>
+  <si>
+    <t>PERSON.BARCODE extend to 16</t>
+  </si>
+  <si>
+    <t>TLOAMASSETGRP</t>
+  </si>
+  <si>
+    <t>STE_CSWNAUTHORITY</t>
   </si>
 </sst>
 </file>
@@ -2071,6 +2083,11 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2085,11 +2102,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3041,18 +3053,18 @@
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="C3" s="72" t="s">
+      <c r="C3" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="74" t="s">
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="75"/>
-      <c r="I3" s="75"/>
-      <c r="J3" s="76"/>
+      <c r="H3" s="78"/>
+      <c r="I3" s="78"/>
+      <c r="J3" s="79"/>
       <c r="K3" s="3" t="s">
         <v>61</v>
       </c>
@@ -10043,10 +10055,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB88DB5-3756-408C-974A-7C21E554649F}">
-  <dimension ref="A1:J71"/>
+  <dimension ref="A1:J75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="D78" sqref="D78"/>
+      <selection activeCell="D75" sqref="D75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -10709,10 +10721,10 @@
         <v>50</v>
       </c>
     </row>
-    <row r="63" spans="1:6" s="78" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="77"/>
-      <c r="E63" s="79"/>
-      <c r="F63" s="79"/>
+    <row r="63" spans="1:6" s="73" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="72"/>
+      <c r="E63" s="74"/>
+      <c r="F63" s="74"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
@@ -10728,7 +10740,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>323</v>
       </c>
@@ -10742,7 +10754,7 @@
         <v>32000</v>
       </c>
     </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>383</v>
       </c>
@@ -10756,7 +10768,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>410</v>
       </c>
@@ -10770,9 +10782,37 @@
         <v>20</v>
       </c>
     </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D71" s="2" t="s">
         <v>412</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" s="73" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="72"/>
+      <c r="D72" s="74"/>
+      <c r="E72" s="74"/>
+      <c r="F72" s="74"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>413</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>415</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="F75" s="2">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- fixed: gldebitacct in prline, rfqline, poline and invoicecost - add timestamp mapping in 01xx and 02xx packages - fixed: JobPlan mapping
</commit_message>
<xml_diff>
--- a/Integration Services Project2/notes/STR(DM-Transaction)-Appendix B - Test and PR Summary.xlsx
+++ b/Integration Services Project2/notes/STR(DM-Transaction)-Appendix B - Test and PR Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\STE.2022.CoswinMigration\Integration Services Project2\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0895AFCF-F764-438C-BE57-B0212AA6906C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{839D1112-6550-4E15-9C0E-AAB1F7B4FE8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="427">
   <si>
     <t>Test Status</t>
   </si>
@@ -1593,9 +1593,6 @@
     <t>TLOAMASSETGRP</t>
   </si>
   <si>
-    <t>STE_CSWNAUTHORITY</t>
-  </si>
-  <si>
     <t>invlot</t>
   </si>
   <si>
@@ -1609,6 +1606,24 @@
   </si>
   <si>
     <t>TIMESTAMP</t>
+  </si>
+  <si>
+    <t>invoicecost</t>
+  </si>
+  <si>
+    <t>invoicecost.gldebitacct extend to 110</t>
+  </si>
+  <si>
+    <t>New custom column: TLOAMASSETGRP.STE_CSWNAUTHORITY</t>
+  </si>
+  <si>
+    <t>invtrans</t>
+  </si>
+  <si>
+    <t>New custom column: INVTRANS.STE_MIGRATIONTS</t>
+  </si>
+  <si>
+    <t>integer</t>
   </si>
 </sst>
 </file>
@@ -10070,10 +10085,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB88DB5-3756-408C-974A-7C21E554649F}">
-  <dimension ref="A1:J78"/>
+  <dimension ref="A1:J82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="D80" sqref="D80"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="D84" sqref="D84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -10821,7 +10836,7 @@
         <v>415</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>318</v>
@@ -10832,21 +10847,40 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
+        <v>416</v>
+      </c>
+      <c r="D77" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="D77" s="2" t="s">
-        <v>418</v>
-      </c>
       <c r="E77" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D78" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E78" s="2" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
         <v>421</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>424</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>426</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed: Chart Of Accounts (not tested)
</commit_message>
<xml_diff>
--- a/Integration Services Project2/notes/STR(DM-Transaction)-Appendix B - Test and PR Summary.xlsx
+++ b/Integration Services Project2/notes/STR(DM-Transaction)-Appendix B - Test and PR Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\STE.2022.CoswinMigration\Integration Services Project2\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{839D1112-6550-4E15-9C0E-AAB1F7B4FE8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59595D43-F0EC-46E7-B2D5-6A65FDFC8636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="432">
   <si>
     <t>Test Status</t>
   </si>
@@ -1624,6 +1624,21 @@
   </si>
   <si>
     <t>integer</t>
+  </si>
+  <si>
+    <t>GLCOMPONENTS</t>
+  </si>
+  <si>
+    <t>New custom column: GLCOMPONENTS.STE_MIGRATIONID</t>
+  </si>
+  <si>
+    <t>New custom column: GLCOMPONENTS.STE_MIGRATIONDATE</t>
+  </si>
+  <si>
+    <t>New custom column: GLCOMPONENTS.STE_MIGRATIONSOURCE</t>
+  </si>
+  <si>
+    <t>New custom column: GLCOMPONENTS.STE_COSTCENTREDEPT</t>
   </si>
 </sst>
 </file>
@@ -10085,10 +10100,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB88DB5-3756-408C-974A-7C21E554649F}">
-  <dimension ref="A1:J82"/>
+  <dimension ref="A1:J87"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="D84" sqref="D84"/>
+      <selection activeCell="E87" sqref="E87:F87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -10872,7 +10887,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>424</v>
       </c>
@@ -10881,6 +10896,47 @@
       </c>
       <c r="E82" s="2" t="s">
         <v>426</v>
+      </c>
+    </row>
+    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>427</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D85" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="86" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D86" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="F86" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="87" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D87" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="F87" s="2">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- tested 00xx and 05xx packages
</commit_message>
<xml_diff>
--- a/Integration Services Project2/notes/STR(DM-Transaction)-Appendix B - Test and PR Summary.xlsx
+++ b/Integration Services Project2/notes/STR(DM-Transaction)-Appendix B - Test and PR Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\STE.2022.CoswinMigration\Integration Services Project2\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59595D43-F0EC-46E7-B2D5-6A65FDFC8636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6BC60DC-DF0F-46C7-A600-6CC4BFC8A2C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="432">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="441">
   <si>
     <t>Test Status</t>
   </si>
@@ -1639,6 +1639,34 @@
   </si>
   <si>
     <t>New custom column: GLCOMPONENTS.STE_COSTCENTREDEPT</t>
+  </si>
+  <si>
+    <t>ITEM</t>
+  </si>
+  <si>
+    <t>New custom column: ITEM.STE_CSWNITEMNO</t>
+  </si>
+  <si>
+    <t>New custom column: ITEM.STE_SPARECRITICAL</t>
+  </si>
+  <si>
+    <t>PERSONANCESTOR</t>
+  </si>
+  <si>
+    <t>New custom column: PERSONANCESTOR.STE_MIGRATIONID</t>
+  </si>
+  <si>
+    <t>New custom column: PERSONANCESTOR.STE_MIGRATIONDATE</t>
+  </si>
+  <si>
+    <t>companies</t>
+  </si>
+  <si>
+    <t>item</t>
+  </si>
+  <si>
+    <t xml:space="preserve">extend ste_itempartno to 60 char
+</t>
   </si>
 </sst>
 </file>
@@ -10100,10 +10128,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB88DB5-3756-408C-974A-7C21E554649F}">
-  <dimension ref="A1:J87"/>
+  <dimension ref="A1:J97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="E87" sqref="E87:F87"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="C94" sqref="C94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -10937,6 +10965,66 @@
       </c>
       <c r="F87" s="2">
         <v>50</v>
+      </c>
+    </row>
+    <row r="89" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>432</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="F89" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="90" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D90" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="F90" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
+        <v>435</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="93" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D93" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="95" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B95" t="s">
+        <v>438</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="97" spans="2:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="B97" t="s">
+        <v>439</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>440</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- fixed: Empty GLCode in GLComponents
</commit_message>
<xml_diff>
--- a/Integration Services Project2/notes/STR(DM-Transaction)-Appendix B - Test and PR Summary.xlsx
+++ b/Integration Services Project2/notes/STR(DM-Transaction)-Appendix B - Test and PR Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\STE.2022.CoswinMigration\Integration Services Project2\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6BC60DC-DF0F-46C7-A600-6CC4BFC8A2C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F395018-B308-43AB-BAEC-FFFCE2866811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="933" uniqueCount="444">
   <si>
     <t>Test Status</t>
   </si>
@@ -1667,6 +1667,16 @@
   <si>
     <t xml:space="preserve">extend ste_itempartno to 60 char
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">extend itemnum to 40 char
+</t>
+  </si>
+  <si>
+    <t>STE_CSWNASSETSLHIST</t>
+  </si>
+  <si>
+    <t>extend STE_CSWNSNO to 30 char</t>
   </si>
 </sst>
 </file>
@@ -10128,10 +10138,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB88DB5-3756-408C-974A-7C21E554649F}">
-  <dimension ref="A1:J97"/>
+  <dimension ref="A1:J100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="C94" sqref="C94"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="D99" sqref="D99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -11025,6 +11035,19 @@
       </c>
       <c r="D97" s="2" t="s">
         <v>440</v>
+      </c>
+    </row>
+    <row r="98" spans="2:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="D98" s="2" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B100" t="s">
+        <v>442</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>443</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Fixed: mapping coswin entity to maint entity - Fixed: mapping invalid CostCenter
</commit_message>
<xml_diff>
--- a/Integration Services Project2/notes/STR(DM-Transaction)-Appendix B - Test and PR Summary.xlsx
+++ b/Integration Services Project2/notes/STR(DM-Transaction)-Appendix B - Test and PR Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\STE.2022.CoswinMigration\Integration Services Project2\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F395018-B308-43AB-BAEC-FFFCE2866811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{375B1382-1B79-4194-8D23-8AA4A42BD554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="933" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="933" uniqueCount="441">
   <si>
     <t>Test Status</t>
   </si>
@@ -1078,9 +1078,6 @@
     <t>Custom column: ste_actualstartdate (date) mapped from PO_VALID_FM</t>
   </si>
   <si>
-    <t>Not mapped yet but derived column exist. Check with gareth!</t>
-  </si>
-  <si>
     <t>Done</t>
   </si>
   <si>
@@ -1659,12 +1656,6 @@
     <t>New custom column: PERSONANCESTOR.STE_MIGRATIONDATE</t>
   </si>
   <si>
-    <t>companies</t>
-  </si>
-  <si>
-    <t>item</t>
-  </si>
-  <si>
     <t xml:space="preserve">extend ste_itempartno to 60 char
 </t>
   </si>
@@ -1683,7 +1674,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1791,6 +1782,12 @@
       <color rgb="FF0000FF"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="11">
@@ -1973,7 +1970,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2185,6 +2182,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4044,10 +4044,10 @@
         <v>276</v>
       </c>
       <c r="P1" s="30" t="s">
+        <v>393</v>
+      </c>
+      <c r="Q1" s="30" t="s">
         <v>394</v>
-      </c>
-      <c r="Q1" s="30" t="s">
-        <v>395</v>
       </c>
       <c r="R1" s="30" t="s">
         <v>53</v>
@@ -4100,16 +4100,16 @@
         <v>230</v>
       </c>
       <c r="N2" s="34" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="O2" s="59" t="s">
         <v>278</v>
       </c>
       <c r="P2" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q2" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R2" s="34"/>
       <c r="S2" s="36"/>
@@ -4139,20 +4139,20 @@
       </c>
       <c r="K3" s="36"/>
       <c r="L3" s="34" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="M3" s="34" t="s">
         <v>231</v>
       </c>
       <c r="N3" s="34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="O3" s="59"/>
       <c r="P3" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q3" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R3" s="34"/>
       <c r="S3" s="36"/>
@@ -4188,14 +4188,14 @@
         <v>133</v>
       </c>
       <c r="N4" s="34" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="O4" s="59"/>
       <c r="P4" s="34" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="Q4" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R4" s="34"/>
       <c r="S4" s="36"/>
@@ -4231,16 +4231,16 @@
         <v>232</v>
       </c>
       <c r="N5" s="34" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="O5" s="59">
         <v>309</v>
       </c>
       <c r="P5" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q5" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R5" s="34"/>
       <c r="S5" s="36"/>
@@ -4278,14 +4278,14 @@
         <v>232</v>
       </c>
       <c r="N6" s="34" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="O6" s="59"/>
       <c r="P6" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q6" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R6" s="34"/>
       <c r="S6" s="36"/>
@@ -4323,16 +4323,16 @@
         <v>135</v>
       </c>
       <c r="N7" s="34" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="O7" s="59" t="s">
         <v>278</v>
       </c>
       <c r="P7" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q7" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R7" s="34"/>
       <c r="S7" s="36"/>
@@ -4368,16 +4368,16 @@
         <v>136</v>
       </c>
       <c r="N8" s="34" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="O8" s="59" t="s">
         <v>278</v>
       </c>
       <c r="P8" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q8" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R8" s="34"/>
       <c r="S8" s="36"/>
@@ -4419,10 +4419,10 @@
         <v>278</v>
       </c>
       <c r="P9" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q9" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R9" s="34"/>
       <c r="S9" s="36"/>
@@ -4458,14 +4458,14 @@
         <v>165</v>
       </c>
       <c r="N10" s="49" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="O10" s="69"/>
       <c r="P10" s="49" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q10" s="49" t="s">
         <v>396</v>
-      </c>
-      <c r="Q10" s="49" t="s">
-        <v>397</v>
       </c>
       <c r="R10" s="45"/>
       <c r="S10" s="44"/>
@@ -4507,10 +4507,10 @@
         <v>278</v>
       </c>
       <c r="P11" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q11" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R11" s="34"/>
       <c r="S11" s="36"/>
@@ -4552,10 +4552,10 @@
         <v>278</v>
       </c>
       <c r="P12" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q12" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R12" s="34"/>
       <c r="S12" s="36"/>
@@ -4591,16 +4591,16 @@
         <v>141</v>
       </c>
       <c r="N13" s="34" t="s">
+        <v>286</v>
+      </c>
+      <c r="O13" s="59" t="s">
         <v>287</v>
       </c>
-      <c r="O13" s="59" t="s">
-        <v>288</v>
-      </c>
       <c r="P13" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q13" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R13" s="34"/>
       <c r="S13" s="36"/>
@@ -4636,14 +4636,14 @@
         <v>142</v>
       </c>
       <c r="N14" s="34" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="O14" s="59"/>
       <c r="P14" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q14" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R14" s="34"/>
       <c r="S14" s="36"/>
@@ -4681,14 +4681,14 @@
         <v>142</v>
       </c>
       <c r="N15" s="34" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="O15" s="59"/>
       <c r="P15" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q15" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R15" s="34"/>
       <c r="S15" s="36"/>
@@ -4726,14 +4726,14 @@
         <v>138</v>
       </c>
       <c r="N16" s="49" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="O16" s="59"/>
       <c r="P16" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q16" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R16" s="34"/>
       <c r="S16" s="36"/>
@@ -4769,14 +4769,14 @@
         <v>144</v>
       </c>
       <c r="N17" s="34" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="O17" s="59"/>
       <c r="P17" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q17" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R17" s="34"/>
       <c r="S17" s="36"/>
@@ -4812,14 +4812,14 @@
         <v>145</v>
       </c>
       <c r="N18" s="32" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="O18" s="60"/>
       <c r="P18" s="32" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q18" s="32" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R18" s="45"/>
       <c r="S18" s="44"/>
@@ -4855,16 +4855,16 @@
         <v>142</v>
       </c>
       <c r="N19" s="34" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="O19" s="59" t="s">
         <v>254</v>
       </c>
       <c r="P19" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q19" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R19" s="45"/>
       <c r="S19" s="44"/>
@@ -4902,14 +4902,14 @@
         <v>146</v>
       </c>
       <c r="N20" s="34" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="O20" s="59"/>
       <c r="P20" s="34" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="Q20" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R20" s="45"/>
       <c r="S20" s="44"/>
@@ -4947,14 +4947,14 @@
         <v>143</v>
       </c>
       <c r="N21" s="49" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="O21" s="59"/>
       <c r="P21" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q21" s="50" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="R21" s="34"/>
       <c r="S21" s="36"/>
@@ -4992,10 +4992,10 @@
       <c r="N22" s="34"/>
       <c r="O22" s="59"/>
       <c r="P22" s="34" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="Q22" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R22" s="45"/>
       <c r="S22" s="44"/>
@@ -5031,14 +5031,14 @@
         <v>149</v>
       </c>
       <c r="N23" s="34" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="O23" s="59"/>
       <c r="P23" s="34" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="Q23" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R23" s="45"/>
       <c r="S23" s="44"/>
@@ -5074,14 +5074,14 @@
         <v>151</v>
       </c>
       <c r="N24" s="34" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="O24" s="59"/>
       <c r="P24" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q24" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R24" s="45"/>
       <c r="S24" s="44"/>
@@ -5117,14 +5117,14 @@
         <v>153</v>
       </c>
       <c r="N25" s="34" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="O25" s="68"/>
       <c r="P25" s="34" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="Q25" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R25" s="45"/>
       <c r="S25" s="44"/>
@@ -5162,14 +5162,14 @@
         <v>159</v>
       </c>
       <c r="N26" s="34" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="O26" s="59"/>
       <c r="P26" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q26" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R26" s="45"/>
       <c r="S26" s="44"/>
@@ -5209,10 +5209,10 @@
       </c>
       <c r="O27" s="59"/>
       <c r="P27" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q27" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R27" s="45"/>
       <c r="S27" s="44"/>
@@ -5248,14 +5248,14 @@
         <v>161</v>
       </c>
       <c r="N28" s="34" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="O28" s="59"/>
       <c r="P28" s="34" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="Q28" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R28" s="45"/>
       <c r="S28" s="44"/>
@@ -5293,14 +5293,14 @@
         <v>147</v>
       </c>
       <c r="N29" s="49" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="O29" s="59"/>
       <c r="P29" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q29" s="50" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="R29" s="45"/>
       <c r="S29" s="44"/>
@@ -5336,14 +5336,14 @@
         <v>232</v>
       </c>
       <c r="N30" s="34" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="O30" s="59"/>
       <c r="P30" s="34" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="Q30" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R30" s="45"/>
       <c r="S30" s="44"/>
@@ -5379,14 +5379,14 @@
         <v>162</v>
       </c>
       <c r="N31" s="49" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="O31" s="59"/>
       <c r="P31" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q31" s="50" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="R31" s="45"/>
       <c r="S31" s="44"/>
@@ -5426,10 +5426,10 @@
       </c>
       <c r="O32" s="59"/>
       <c r="P32" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q32" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R32" s="45"/>
       <c r="S32" s="44"/>
@@ -5465,14 +5465,14 @@
         <v>162</v>
       </c>
       <c r="N33" s="34" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="O33" s="59"/>
       <c r="P33" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q33" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R33" s="45"/>
       <c r="S33" s="44"/>
@@ -5508,14 +5508,14 @@
         <v>162</v>
       </c>
       <c r="N34" s="34" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="O34" s="59"/>
       <c r="P34" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q34" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R34" s="45"/>
       <c r="S34" s="44"/>
@@ -5555,10 +5555,10 @@
       </c>
       <c r="O35" s="59"/>
       <c r="P35" s="34" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="Q35" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R35" s="45"/>
       <c r="S35" s="44"/>
@@ -5598,10 +5598,10 @@
       </c>
       <c r="O36" s="59"/>
       <c r="P36" s="34" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="Q36" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R36" s="45"/>
       <c r="S36" s="44"/>
@@ -5637,14 +5637,14 @@
         <v>170</v>
       </c>
       <c r="N37" s="34" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="O37" s="59"/>
       <c r="P37" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q37" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R37" s="45"/>
       <c r="S37" s="44"/>
@@ -5684,10 +5684,10 @@
       </c>
       <c r="O38" s="59"/>
       <c r="P38" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q38" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R38" s="45"/>
       <c r="S38" s="44"/>
@@ -5725,10 +5725,10 @@
       <c r="N39" s="34"/>
       <c r="O39" s="59"/>
       <c r="P39" s="34" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="Q39" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R39" s="45"/>
       <c r="S39" s="44"/>
@@ -5768,10 +5768,10 @@
       </c>
       <c r="O40" s="59"/>
       <c r="P40" s="34" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="Q40" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R40" s="45"/>
       <c r="S40" s="44"/>
@@ -5813,10 +5813,10 @@
       </c>
       <c r="O41" s="59"/>
       <c r="P41" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q41" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R41" s="45"/>
       <c r="S41" s="44"/>
@@ -5852,14 +5852,14 @@
         <v>211</v>
       </c>
       <c r="N42" s="49" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="O42" s="59"/>
       <c r="P42" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q42" s="50" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="R42" s="45"/>
       <c r="S42" s="44"/>
@@ -5899,10 +5899,10 @@
       </c>
       <c r="O43" s="59"/>
       <c r="P43" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q43" s="50" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="R43" s="45"/>
       <c r="S43" s="44"/>
@@ -5944,10 +5944,10 @@
       </c>
       <c r="O44" s="59"/>
       <c r="P44" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q44" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R44" s="45"/>
       <c r="S44" s="44"/>
@@ -5985,10 +5985,10 @@
       <c r="N45" s="34"/>
       <c r="O45" s="59"/>
       <c r="P45" s="34" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="Q45" s="34" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="R45" s="45"/>
       <c r="S45" s="44"/>
@@ -6026,10 +6026,10 @@
       <c r="N46" s="34"/>
       <c r="O46" s="59"/>
       <c r="P46" s="34" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="Q46" s="34" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="R46" s="45"/>
       <c r="S46" s="44"/>
@@ -6069,10 +6069,10 @@
       <c r="N47" s="34"/>
       <c r="O47" s="59"/>
       <c r="P47" s="34" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="Q47" s="34" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="R47" s="45"/>
       <c r="S47" s="44"/>
@@ -6112,10 +6112,10 @@
       <c r="N48" s="34"/>
       <c r="O48" s="59"/>
       <c r="P48" s="34" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="Q48" s="34" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="R48" s="45"/>
       <c r="S48" s="44"/>
@@ -6153,10 +6153,10 @@
       <c r="N49" s="34"/>
       <c r="O49" s="59"/>
       <c r="P49" s="34" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="Q49" s="34" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="R49" s="45"/>
       <c r="S49" s="44"/>
@@ -6196,10 +6196,10 @@
       <c r="N50" s="34"/>
       <c r="O50" s="59"/>
       <c r="P50" s="34" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="Q50" s="34" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="R50" s="45"/>
       <c r="S50" s="44"/>
@@ -6239,10 +6239,10 @@
       <c r="N51" s="34"/>
       <c r="O51" s="59"/>
       <c r="P51" s="34" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="Q51" s="34" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="R51" s="45"/>
       <c r="S51" s="44"/>
@@ -6280,10 +6280,10 @@
       <c r="N52" s="34"/>
       <c r="O52" s="59"/>
       <c r="P52" s="34" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="Q52" s="34" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="R52" s="45"/>
       <c r="S52" s="44"/>
@@ -6323,10 +6323,10 @@
       <c r="N53" s="34"/>
       <c r="O53" s="59"/>
       <c r="P53" s="34" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="Q53" s="34" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="R53" s="45"/>
       <c r="S53" s="44"/>
@@ -6364,10 +6364,10 @@
       <c r="N54" s="34"/>
       <c r="O54" s="59"/>
       <c r="P54" s="34" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="Q54" s="34" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="R54" s="45"/>
       <c r="S54" s="44"/>
@@ -6407,10 +6407,10 @@
       <c r="N55" s="34"/>
       <c r="O55" s="59"/>
       <c r="P55" s="34" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="Q55" s="34" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="R55" s="45"/>
       <c r="S55" s="44"/>
@@ -6450,10 +6450,10 @@
       <c r="N56" s="34"/>
       <c r="O56" s="59"/>
       <c r="P56" s="34" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="Q56" s="34" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="R56" s="45"/>
       <c r="S56" s="44"/>
@@ -6493,10 +6493,10 @@
       <c r="N57" s="34"/>
       <c r="O57" s="59"/>
       <c r="P57" s="34" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="Q57" s="34" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="R57" s="45"/>
       <c r="S57" s="44"/>
@@ -6534,10 +6534,10 @@
       <c r="N58" s="34"/>
       <c r="O58" s="59"/>
       <c r="P58" s="34" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="Q58" s="34" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="R58" s="45"/>
       <c r="S58" s="44"/>
@@ -6573,14 +6573,14 @@
         <v>211</v>
       </c>
       <c r="N59" s="34" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="O59" s="59"/>
       <c r="P59" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q59" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R59" s="45"/>
       <c r="S59" s="44"/>
@@ -6616,14 +6616,14 @@
         <v>221</v>
       </c>
       <c r="N60" s="34" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="O60" s="59"/>
       <c r="P60" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q60" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R60" s="45"/>
       <c r="S60" s="44"/>
@@ -6659,14 +6659,14 @@
         <v>211</v>
       </c>
       <c r="N61" s="34" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="O61" s="59"/>
       <c r="P61" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q61" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R61" s="45"/>
       <c r="S61" s="44"/>
@@ -6702,14 +6702,14 @@
         <v>211</v>
       </c>
       <c r="N62" s="34" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="O62" s="59"/>
       <c r="P62" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q62" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R62" s="45"/>
       <c r="S62" s="44"/>
@@ -6745,14 +6745,14 @@
         <v>211</v>
       </c>
       <c r="N63" s="34" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="O63" s="59"/>
       <c r="P63" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q63" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R63" s="45"/>
       <c r="S63" s="44"/>
@@ -6790,14 +6790,14 @@
         <v>211</v>
       </c>
       <c r="N64" s="34" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="O64" s="59"/>
       <c r="P64" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q64" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R64" s="45"/>
       <c r="S64" s="44"/>
@@ -6835,14 +6835,14 @@
         <v>211</v>
       </c>
       <c r="N65" s="34" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="O65" s="59"/>
       <c r="P65" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q65" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R65" s="45"/>
       <c r="S65" s="44"/>
@@ -6874,20 +6874,20 @@
       </c>
       <c r="K66" s="34"/>
       <c r="L66" s="34" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="M66" s="34" t="s">
         <v>211</v>
       </c>
       <c r="N66" s="49" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="O66" s="59"/>
       <c r="P66" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q66" s="50" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="R66" s="45"/>
       <c r="S66" s="44"/>
@@ -6925,14 +6925,14 @@
         <v>211</v>
       </c>
       <c r="N67" s="63" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="O67" s="55"/>
       <c r="P67" s="34" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="Q67" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R67" s="45"/>
       <c r="S67" s="44"/>
@@ -6968,14 +6968,14 @@
         <v>211</v>
       </c>
       <c r="N68" s="34" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="O68" s="59"/>
       <c r="P68" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q68" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R68" s="45"/>
       <c r="S68" s="44"/>
@@ -7011,14 +7011,14 @@
         <v>211</v>
       </c>
       <c r="N69" s="34" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="O69" s="59"/>
       <c r="P69" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q69" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R69" s="45"/>
       <c r="S69" s="44"/>
@@ -7058,10 +7058,10 @@
       </c>
       <c r="O70" s="59"/>
       <c r="P70" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q70" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R70" s="45"/>
       <c r="S70" s="44"/>
@@ -7097,14 +7097,14 @@
         <v>211</v>
       </c>
       <c r="N71" s="34" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="O71" s="59"/>
       <c r="P71" s="34" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="Q71" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R71" s="45"/>
       <c r="S71" s="44"/>
@@ -7140,14 +7140,14 @@
         <v>211</v>
       </c>
       <c r="N72" s="49" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O72" s="59"/>
       <c r="P72" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q72" s="50" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="R72" s="45"/>
       <c r="S72" s="44"/>
@@ -7170,7 +7170,7 @@
         <v>246</v>
       </c>
       <c r="I73" s="48" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="J73" s="33" t="s">
         <v>121</v>
@@ -7189,10 +7189,10 @@
       </c>
       <c r="O73" s="59"/>
       <c r="P73" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q73" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R73" s="45"/>
       <c r="S73" s="44"/>
@@ -7228,14 +7228,14 @@
         <v>211</v>
       </c>
       <c r="N74" s="34" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="O74" s="59"/>
       <c r="P74" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q74" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R74" s="45"/>
       <c r="S74" s="44"/>
@@ -7271,14 +7271,14 @@
         <v>211</v>
       </c>
       <c r="N75" s="49" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="O75" s="59"/>
       <c r="P75" s="49" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="Q75" s="50" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="R75" s="45"/>
       <c r="S75" s="44"/>
@@ -7314,14 +7314,14 @@
         <v>211</v>
       </c>
       <c r="N76" s="34" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="O76" s="59"/>
       <c r="P76" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q76" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R76" s="45"/>
       <c r="S76" s="44"/>
@@ -7363,10 +7363,10 @@
         <v>206</v>
       </c>
       <c r="P77" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q77" s="50" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="R77" s="45"/>
       <c r="S77" s="44"/>
@@ -10138,10 +10138,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB88DB5-3756-408C-974A-7C21E554649F}">
-  <dimension ref="A1:J100"/>
+  <dimension ref="A1:J98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="D99" sqref="D99"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -10169,10 +10169,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D2" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F2" s="2">
         <v>20</v>
@@ -10202,10 +10202,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D6" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F6" s="2">
         <v>20</v>
@@ -10213,10 +10213,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D7" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F7" s="2">
         <v>20</v>
@@ -10224,10 +10224,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D8" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F8" s="2">
         <v>16</v>
@@ -10235,10 +10235,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D9" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F9" s="2">
         <v>12</v>
@@ -10246,16 +10246,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D10" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="F10" s="2">
-        <v>32000</v>
-      </c>
-      <c r="G10" t="s">
-        <v>313</v>
+        <v>317</v>
+      </c>
+      <c r="F10" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -10271,16 +10268,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D13" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="F13" s="2">
-        <v>32000</v>
-      </c>
-      <c r="G13" t="s">
-        <v>313</v>
+        <v>317</v>
+      </c>
+      <c r="F13" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
@@ -10296,32 +10290,29 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D16" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D17" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="F17" s="2">
-        <v>32000</v>
-      </c>
-      <c r="G17" t="s">
-        <v>313</v>
+        <v>317</v>
+      </c>
+      <c r="F17" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
       <c r="D18" s="19" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E18" s="64" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F18" s="55">
         <v>16</v>
@@ -10335,48 +10326,42 @@
         <v>279</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D21" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="80" t="s">
         <v>280</v>
-      </c>
-      <c r="G22" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D23" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="F23" s="2">
-        <v>32000</v>
-      </c>
-      <c r="G23" t="s">
-        <v>313</v>
+        <v>317</v>
+      </c>
+      <c r="F23" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D24" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F24" s="2">
         <v>110</v>
@@ -10384,16 +10369,16 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="56" t="s">
+        <v>297</v>
+      </c>
+      <c r="B26" t="s">
         <v>298</v>
       </c>
-      <c r="B26" t="s">
-        <v>299</v>
-      </c>
       <c r="D26" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F26" s="2">
         <v>12</v>
@@ -10401,16 +10386,16 @@
     </row>
     <row r="28" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A28" s="56" t="s">
+        <v>320</v>
+      </c>
+      <c r="B28" t="s">
         <v>321</v>
       </c>
-      <c r="B28" t="s">
-        <v>322</v>
-      </c>
       <c r="D28" s="19" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E28" s="64" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F28" s="55">
         <v>16</v>
@@ -10420,10 +10405,10 @@
     </row>
     <row r="29" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
       <c r="D29" s="64" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E29" s="64" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F29" s="55">
         <v>10</v>
@@ -10433,42 +10418,42 @@
     </row>
     <row r="30" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
       <c r="D30" s="64" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E30" s="64" t="s">
+        <v>318</v>
+      </c>
+      <c r="F30" s="55" t="s">
         <v>319</v>
-      </c>
-      <c r="F30" s="55" t="s">
-        <v>320</v>
       </c>
       <c r="G30" s="64"/>
       <c r="H30" s="55"/>
     </row>
     <row r="31" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
       <c r="D31" s="64" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E31" s="64" t="s">
+        <v>318</v>
+      </c>
+      <c r="F31" s="55" t="s">
         <v>319</v>
-      </c>
-      <c r="F31" s="55" t="s">
-        <v>320</v>
       </c>
       <c r="G31" s="64"/>
       <c r="H31" s="55"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="56" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B33" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D33" s="19" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E33" s="65" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F33" s="32">
         <v>16</v>
@@ -10480,10 +10465,10 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D34" s="19" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E34" s="19" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F34" s="66">
         <v>20</v>
@@ -10495,10 +10480,10 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D35" s="19" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E35" s="65" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F35" s="32">
         <v>10</v>
@@ -10510,10 +10495,10 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E36" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F36" s="67">
         <v>15</v>
@@ -10522,10 +10507,10 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D37" s="19" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E37" s="65" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F37" s="32">
         <v>10</v>
@@ -10537,10 +10522,10 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D38" s="19" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E38" s="65" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F38" s="32">
         <v>10</v>
@@ -10552,10 +10537,10 @@
     </row>
     <row r="39" spans="1:10" ht="14.4" x14ac:dyDescent="0.25">
       <c r="D39" s="64" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E39" s="64" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F39" s="64">
         <v>10</v>
@@ -10567,10 +10552,10 @@
     </row>
     <row r="40" spans="1:10" ht="14.4" x14ac:dyDescent="0.25">
       <c r="D40" s="64" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E40" s="64" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F40" s="64">
         <v>20</v>
@@ -10582,10 +10567,10 @@
     </row>
     <row r="41" spans="1:10" ht="14.4" x14ac:dyDescent="0.25">
       <c r="D41" s="64" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E41" s="64" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F41" s="64">
         <v>10</v>
@@ -10597,10 +10582,10 @@
     </row>
     <row r="42" spans="1:10" ht="14.4" x14ac:dyDescent="0.25">
       <c r="D42" s="64" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E42" s="64" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F42" s="64">
         <v>10</v>
@@ -10612,10 +10597,10 @@
     </row>
     <row r="43" spans="1:10" ht="14.4" x14ac:dyDescent="0.25">
       <c r="D43" s="64" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E43" s="64" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="F43" s="64">
         <v>3</v>
@@ -10627,10 +10612,10 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D44" s="19" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E44" s="65" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F44" s="32">
         <v>3</v>
@@ -10642,10 +10627,10 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E45" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F45" s="67">
         <v>10</v>
@@ -10654,10 +10639,10 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D46" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E46" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F46" s="67">
         <v>15</v>
@@ -10666,10 +10651,10 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D47" s="19" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E47" s="65" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F47" s="32">
         <v>3</v>
@@ -10681,24 +10666,24 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D48" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="F48" s="2">
-        <v>32000</v>
+        <v>317</v>
+      </c>
+      <c r="F48" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
+        <v>361</v>
+      </c>
+      <c r="D50" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="D50" s="2" t="s">
-        <v>363</v>
-      </c>
       <c r="E50" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F50" s="2">
         <v>20</v>
@@ -10706,46 +10691,46 @@
     </row>
     <row r="52" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D52" s="64" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E52" s="64" t="s">
+        <v>318</v>
+      </c>
+      <c r="F52" s="55" t="s">
         <v>319</v>
-      </c>
-      <c r="F52" s="55" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
       <c r="D53" s="64" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E53" s="64" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F53" s="55" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
       <c r="D54" s="64" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E54" s="64" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F54" s="55" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
       <c r="D55" s="64" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E55" s="64" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F55" s="55">
         <v>20</v>
@@ -10753,24 +10738,24 @@
     </row>
     <row r="56" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
       <c r="D56" s="64" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E56" s="64" t="s">
+        <v>318</v>
+      </c>
+      <c r="F56" s="55" t="s">
         <v>319</v>
-      </c>
-      <c r="F56" s="55" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D58" t="s">
         <v>249</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F58" s="2">
         <v>8</v>
@@ -10778,27 +10763,27 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
+        <v>382</v>
+      </c>
+      <c r="D60" t="s">
         <v>383</v>
       </c>
-      <c r="D60" t="s">
-        <v>384</v>
-      </c>
       <c r="E60" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="F60" s="2">
-        <v>32000</v>
+        <v>317</v>
+      </c>
+      <c r="F60" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
+        <v>384</v>
+      </c>
+      <c r="D62" t="s">
         <v>385</v>
       </c>
-      <c r="D62" t="s">
-        <v>386</v>
-      </c>
       <c r="E62" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F62" s="2">
         <v>50</v>
@@ -10811,13 +10796,13 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
+        <v>405</v>
+      </c>
+      <c r="D64" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="D64" s="2" t="s">
-        <v>407</v>
-      </c>
       <c r="E64" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F64" s="2">
         <v>50</v>
@@ -10825,27 +10810,27 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D66" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="F66" s="2">
-        <v>32000</v>
+        <v>317</v>
+      </c>
+      <c r="F66" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F68" s="2">
         <v>50</v>
@@ -10853,13 +10838,13 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
+        <v>409</v>
+      </c>
+      <c r="D70" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="D70" s="2" t="s">
-        <v>411</v>
-      </c>
       <c r="E70" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F70" s="2">
         <v>20</v>
@@ -10867,7 +10852,7 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D71" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="72" spans="1:6" s="73" customFormat="1" x14ac:dyDescent="0.25">
@@ -10878,21 +10863,21 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
+        <v>412</v>
+      </c>
+      <c r="D73" s="2" t="s">
         <v>413</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F75" s="2">
         <v>16</v>
@@ -10900,67 +10885,67 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
+        <v>415</v>
+      </c>
+      <c r="D77" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="D77" s="2" t="s">
-        <v>417</v>
-      </c>
       <c r="E77" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D78" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
+        <v>420</v>
+      </c>
+      <c r="D80" s="2" t="s">
         <v>421</v>
-      </c>
-      <c r="D80" s="2" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="82" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
+        <v>423</v>
+      </c>
+      <c r="D82" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="D82" s="2" t="s">
+      <c r="E82" s="2" t="s">
         <v>425</v>
-      </c>
-      <c r="E82" s="2" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="84" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
+        <v>426</v>
+      </c>
+      <c r="D84" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="D84" s="2" t="s">
-        <v>428</v>
-      </c>
       <c r="E84" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="85" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D85" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="86" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D86" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F86" s="2">
         <v>50</v>
@@ -10968,10 +10953,10 @@
     </row>
     <row r="87" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D87" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F87" s="2">
         <v>50</v>
@@ -10979,13 +10964,13 @@
     </row>
     <row r="89" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
+        <v>431</v>
+      </c>
+      <c r="D89" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="D89" s="2" t="s">
-        <v>433</v>
-      </c>
       <c r="E89" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F89" s="2">
         <v>30</v>
@@ -10993,10 +10978,10 @@
     </row>
     <row r="90" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D90" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F90" s="2">
         <v>2</v>
@@ -11004,50 +10989,42 @@
     </row>
     <row r="92" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
+        <v>434</v>
+      </c>
+      <c r="D92" s="2" t="s">
         <v>435</v>
       </c>
-      <c r="D92" s="2" t="s">
-        <v>436</v>
-      </c>
       <c r="E92" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="93" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D93" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="95" spans="2:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="B95" t="s">
+        <v>431</v>
+      </c>
+      <c r="D95" s="80" t="s">
         <v>437</v>
       </c>
-      <c r="E93" s="2" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="95" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B95" t="s">
+    </row>
+    <row r="96" spans="2:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="D96" s="80" t="s">
         <v>438</v>
       </c>
-      <c r="D95" s="2" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="97" spans="2:4" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B97" t="s">
+    </row>
+    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B98" t="s">
         <v>439</v>
       </c>
-      <c r="D97" s="2" t="s">
+      <c r="D98" s="80" t="s">
         <v>440</v>
-      </c>
-    </row>
-    <row r="98" spans="2:4" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="D98" s="2" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B100" t="s">
-        <v>442</v>
-      </c>
-      <c r="D100" s="2" t="s">
-        <v>443</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Fixed: Timestamp for delta migration
</commit_message>
<xml_diff>
--- a/Integration Services Project2/notes/STR(DM-Transaction)-Appendix B - Test and PR Summary.xlsx
+++ b/Integration Services Project2/notes/STR(DM-Transaction)-Appendix B - Test and PR Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\STE.2022.CoswinMigration\Integration Services Project2\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{375B1382-1B79-4194-8D23-8AA4A42BD554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B3151D-1346-4D96-A4DA-31ECF6A3240D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="933" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="442">
   <si>
     <t>Test Status</t>
   </si>
@@ -1668,6 +1668,9 @@
   </si>
   <si>
     <t>extend STE_CSWNSNO to 30 char</t>
+  </si>
+  <si>
+    <t>New custom column: INVENTORY.STE_FIRSTPROCDATE</t>
   </si>
 </sst>
 </file>
@@ -2168,6 +2171,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2182,9 +2188,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3136,18 +3139,18 @@
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="C3" s="75" t="s">
+      <c r="C3" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="77" t="s">
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="77"/>
+      <c r="G3" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78"/>
-      <c r="J3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="80"/>
       <c r="K3" s="3" t="s">
         <v>61</v>
       </c>
@@ -10138,10 +10141,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB88DB5-3756-408C-974A-7C21E554649F}">
-  <dimension ref="A1:J98"/>
+  <dimension ref="A1:J102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -10341,7 +10344,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D22" s="80" t="s">
+      <c r="D22" s="75" t="s">
         <v>280</v>
       </c>
     </row>
@@ -11010,21 +11013,40 @@
       <c r="B95" t="s">
         <v>431</v>
       </c>
-      <c r="D95" s="80" t="s">
+      <c r="D95" s="75" t="s">
         <v>437</v>
       </c>
     </row>
     <row r="96" spans="2:6" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="D96" s="80" t="s">
+      <c r="D96" s="75" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
         <v>439</v>
       </c>
-      <c r="D98" s="80" t="s">
+      <c r="D98" s="75" t="s">
         <v>440</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" s="72"/>
+      <c r="B100" s="73"/>
+      <c r="C100" s="73"/>
+      <c r="D100" s="74"/>
+      <c r="E100" s="74"/>
+      <c r="F100" s="74"/>
+    </row>
+    <row r="102" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B102" t="s">
+        <v>365</v>
+      </c>
+      <c r="D102" s="64" t="s">
+        <v>441</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>419</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
0006-Master-Item - Add mapping for missing columns: STE_CSWNMAINSTORE, STE_ITEMGROUP, STE_CSWNITEMDECIMAL
0307-PO-Invoice
- Add mapping for missing column: STE_CSWNINVADJSTATUS

0401-WO-Workorder
- Add df for route workorder

0405-WO-SR
- Move mapping for origrecordid to 0407-WO-RelatedRecord

0407-WO-RelatedRecord
- Update SR and WO relationship
- Log nomatch relationship between SR and WO
</commit_message>
<xml_diff>
--- a/Integration Services Project2/notes/STR(DM-Transaction)-Appendix B - Test and PR Summary.xlsx
+++ b/Integration Services Project2/notes/STR(DM-Transaction)-Appendix B - Test and PR Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\STE.2022.CoswinMigration\Integration Services Project2\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{998D2760-B3CE-4422-990B-330F9E6BCA4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5AF7B62-A8F0-4C47-B8E9-B955BB65B8CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3648" yWindow="3288" windowWidth="17280" windowHeight="8880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Summary" sheetId="6" r:id="rId1"/>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="455">
   <si>
     <t>Test Status</t>
   </si>
@@ -1690,12 +1690,765 @@
   <si>
     <t>RFQ.STE_MIGRATIONTS</t>
   </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>PLUSTMTRCHNG</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF006464"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONID"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>BIGINT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>PLUSTMTRCHNG</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF006464"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONDATE"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TIMESTAMP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>PLUSTMTRCHNG</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF006464"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONTS"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>INTEGER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <t>-- PLUSTMTRCHNG</t>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>PLUSTASSETSTHIST</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF006464"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONID"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>BIGINT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>PLUSTASSETSTHIST</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF006464"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONDATE"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TIMESTAMP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>PLUSTASSETSTHIST</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF006464"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONTS"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>INTEGER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1810,8 +2563,46 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF800000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF6C5151"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000080"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1869,6 +2660,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1991,7 +2788,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2206,6 +3003,20 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -10159,10 +10970,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB88DB5-3756-408C-974A-7C21E554649F}">
-  <dimension ref="A1:J107"/>
+  <dimension ref="A1:J119"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="A101" sqref="A101:E108"/>
+      <selection activeCell="B113" sqref="B113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -11095,6 +11906,57 @@
       </c>
       <c r="E107" s="2" t="s">
         <v>444</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A109" s="81"/>
+      <c r="B109" s="82"/>
+      <c r="C109" s="82"/>
+      <c r="D109" s="83"/>
+      <c r="E109" s="83"/>
+      <c r="F109" s="83"/>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B111" s="86" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B112" s="84" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B113" s="84" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B114" s="84" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B115" s="85"/>
+    </row>
+    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B116" s="86" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B117" s="84" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="118" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B118" s="84" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B119" s="84" t="s">
+        <v>454</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
After data-integrity and completeness analysis
</commit_message>
<xml_diff>
--- a/Integration Services Project2/notes/STR(DM-Transaction)-Appendix B - Test and PR Summary.xlsx
+++ b/Integration Services Project2/notes/STR(DM-Transaction)-Appendix B - Test and PR Summary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\STE.2022.CoswinMigration\Integration Services Project2\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5AF7B62-A8F0-4C47-B8E9-B955BB65B8CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{441B1688-A3BF-442A-858C-CFAA3083A03C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="456">
   <si>
     <t>Test Status</t>
   </si>
@@ -2443,12 +2443,164 @@
       <t>;</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF956037"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF8E00C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>AMCREW</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONSOURCE"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>VARCHAR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>50</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2598,6 +2750,18 @@
     <font>
       <sz val="10"/>
       <color rgb="FF808080"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF956037"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF8E00C6"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
@@ -2788,7 +2952,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2989,6 +3153,20 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="19" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3004,20 +3182,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3968,18 +4133,18 @@
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="C3" s="76" t="s">
+      <c r="C3" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="77"/>
-      <c r="G3" s="78" t="s">
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="83"/>
+      <c r="G3" s="84" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="79"/>
-      <c r="I3" s="79"/>
-      <c r="J3" s="80"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="86"/>
       <c r="K3" s="3" t="s">
         <v>61</v>
       </c>
@@ -10970,10 +11135,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB88DB5-3756-408C-974A-7C21E554649F}">
-  <dimension ref="A1:J119"/>
+  <dimension ref="A1:J123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="B113" sqref="B113"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="B123" sqref="B123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -11909,54 +12074,65 @@
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A109" s="81"/>
-      <c r="B109" s="82"/>
-      <c r="C109" s="82"/>
-      <c r="D109" s="83"/>
-      <c r="E109" s="83"/>
-      <c r="F109" s="83"/>
+      <c r="A109" s="76"/>
+      <c r="B109" s="77"/>
+      <c r="C109" s="77"/>
+      <c r="D109" s="78"/>
+      <c r="E109" s="78"/>
+      <c r="F109" s="78"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B111" s="86" t="s">
+      <c r="B111" s="81" t="s">
         <v>451</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B112" s="84" t="s">
+      <c r="B112" s="79" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B113" s="84" t="s">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B113" s="79" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B114" s="84" t="s">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B114" s="79" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B115" s="85"/>
-    </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B116" s="86" t="s">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B115" s="80"/>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B116" s="81" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B117" s="84" t="s">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B117" s="79" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B118" s="84" t="s">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B118" s="79" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B119" s="84" t="s">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B119" s="79" t="s">
         <v>454</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" s="73" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="72"/>
+      <c r="D121" s="74"/>
+      <c r="E121" s="74"/>
+      <c r="F121" s="74"/>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B123" s="87" t="s">
+        <v>455</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Add 0311-PO-STE_CSWNRECEIPT_PER_CC: accepted qty per costcenter
0012-Master-GLComponents:
- Add SAPGL from RECEIPT
- Clean up empty/single char SAPGL
- Use uppercase for SAPGL

0205-MR-MRLine:
- Add new mapping MR.STE_CSWNDEMTYPE

0303-PO-PR-PRLine-PRCost:
- Use uppercase for SAPGL in PRLine

0304-PO-RFQ-RFQLine:
- Use uppercase for SAPGL in RFQLine

0306-PO-PO-POLine-POCost:
- Use uppercase for SAPGL in POLine

0303-PO-Invoice-InvoiceLine-InvoiceCost:
- Use uppercase for SAPGL in InvoiceCost

0308-PO-MATRECTRANS-SERVRECTRANS:
- Add new mapping STE_CSWNACPQTY
- Add new mapping STE_CSWNRTNTOSUPL
- Set rejectqty to RTN_TO_SUPL when it is non-zero. Otherwise, rejectqty = RCT_QTY - ACP_QTY

0901-Post-MAXDOMAIN-Validation:
- Execute SP MIGRATION.STE_VALIDATE_MAXDOMAIN
</commit_message>
<xml_diff>
--- a/Integration Services Project2/notes/STR(DM-Transaction)-Appendix B - Test and PR Summary.xlsx
+++ b/Integration Services Project2/notes/STR(DM-Transaction)-Appendix B - Test and PR Summary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\STE.2022.CoswinMigration\Integration Services Project2\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{441B1688-A3BF-442A-858C-CFAA3083A03C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B19F3B4D-3EB9-42E6-A13C-9A63871BE75C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,11 +16,12 @@
     <sheet name="Test Summary" sheetId="6" r:id="rId1"/>
     <sheet name="PR Summary" sheetId="14" r:id="rId2"/>
     <sheet name="Custom Column" sheetId="15" r:id="rId3"/>
-    <sheet name="Drop down list" sheetId="12" state="hidden" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="16" r:id="rId4"/>
+    <sheet name="Drop down list" sheetId="12" state="hidden" r:id="rId5"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId5"/>
     <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'PR Summary'!$A$1:$Y$77</definedName>
@@ -100,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="468">
   <si>
     <t>Test Status</t>
   </si>
@@ -2584,6 +2585,1425 @@
         <family val="3"/>
       </rPr>
       <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF956037"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO.MATRECTRANS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_CSWNACPQTY"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>DECIMAL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(15,2)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF956037"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO.MATRECTRANS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_CSWNRTNTOSUPL"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>DECIMAL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(15,2)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF956037"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO.SERVRECTRANS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_CSWNACPQTY"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>DECIMAL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(15,2)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF956037"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO.SERVRECTRANS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_CSWNRTNTOSUPL"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>DECIMAL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(15,2)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ALNDOMAIN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF006464"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONID"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>BIGINT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ALNDOMAIN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF006464"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONDATE"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TIMESTAMP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ALNDOMAIN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF006464"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONSOURCE"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>VARCHAR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>50</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> MAXIMO.ALNDOMAIN </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF006464"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONTS"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>INTEGER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF956037"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO.MATRECTRANS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_CSWNRCTQTY"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>DECIMAL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(15,2)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF956037"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO.SERVRECTRANS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_CSWNRCTQTY"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>DECIMAL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(15,2)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF956037"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO.MATRECTRANS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_CSWNRCTVAL"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>DECIMAL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(13,5)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF956037"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO.SERVRECTRANS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_CSWNRCTVAL"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>DECIMAL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(13,5)</t>
     </r>
     <r>
       <rPr>
@@ -3167,6 +4587,7 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3182,7 +4603,6 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4133,18 +5553,18 @@
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="C3" s="82" t="s">
+      <c r="C3" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="82"/>
-      <c r="E3" s="82"/>
-      <c r="F3" s="83"/>
-      <c r="G3" s="84" t="s">
+      <c r="D3" s="83"/>
+      <c r="E3" s="83"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="85" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="86"/>
+      <c r="H3" s="86"/>
+      <c r="I3" s="86"/>
+      <c r="J3" s="87"/>
       <c r="K3" s="3" t="s">
         <v>61</v>
       </c>
@@ -11135,10 +12555,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB88DB5-3756-408C-974A-7C21E554649F}">
-  <dimension ref="A1:J123"/>
+  <dimension ref="A1:J139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="B123" sqref="B123"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="C132" sqref="C132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -12131,8 +13551,74 @@
       <c r="F121" s="74"/>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B123" s="87" t="s">
+      <c r="B123" s="82" t="s">
         <v>455</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" s="73" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="72"/>
+      <c r="D125" s="74"/>
+      <c r="E125" s="74"/>
+      <c r="F125" s="74"/>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B127" s="82" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B128" s="82" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="129" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B129" s="82" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="130" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B130" s="82" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B131" s="82" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B132" s="82" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="133" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B133" s="82" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="134" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B134" s="82" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B136" s="79" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="137" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B137" s="79" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="138" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B138" s="79" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="139" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B139" s="79" t="s">
+        <v>463</v>
       </c>
     </row>
   </sheetData>
@@ -12141,6 +13627,437 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FB0FA25-43E2-4113-AAE9-BB13F1213158}">
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>10981</v>
+      </c>
+      <c r="B1">
+        <v>9381</v>
+      </c>
+      <c r="C1">
+        <v>2621101</v>
+      </c>
+      <c r="D1">
+        <v>4</v>
+      </c>
+      <c r="E1">
+        <v>50</v>
+      </c>
+      <c r="F1">
+        <v>50</v>
+      </c>
+      <c r="G1">
+        <v>0</v>
+      </c>
+      <c r="H1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>10981</v>
+      </c>
+      <c r="B2">
+        <v>9382</v>
+      </c>
+      <c r="C2">
+        <v>2621102</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>50</v>
+      </c>
+      <c r="F2">
+        <v>50</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>10981</v>
+      </c>
+      <c r="B3">
+        <v>9383</v>
+      </c>
+      <c r="C3">
+        <v>2621103</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>50</v>
+      </c>
+      <c r="F3">
+        <v>50</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>10981</v>
+      </c>
+      <c r="B4">
+        <v>9384</v>
+      </c>
+      <c r="C4">
+        <v>2621104</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>50</v>
+      </c>
+      <c r="F4">
+        <v>50</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>10981</v>
+      </c>
+      <c r="B5">
+        <v>9385</v>
+      </c>
+      <c r="C5">
+        <v>2621105</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>50</v>
+      </c>
+      <c r="F5">
+        <v>50</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>10981</v>
+      </c>
+      <c r="B6">
+        <v>9386</v>
+      </c>
+      <c r="C6">
+        <v>2621106</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>50</v>
+      </c>
+      <c r="F6">
+        <v>50</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>10981</v>
+      </c>
+      <c r="B7">
+        <v>9387</v>
+      </c>
+      <c r="C7">
+        <v>2621107</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>50</v>
+      </c>
+      <c r="F7">
+        <v>50</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>10981</v>
+      </c>
+      <c r="B8">
+        <v>9388</v>
+      </c>
+      <c r="C8">
+        <v>2621108</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>50</v>
+      </c>
+      <c r="F8">
+        <v>50</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>10981</v>
+      </c>
+      <c r="B9">
+        <v>9389</v>
+      </c>
+      <c r="C9">
+        <v>2621109</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>50</v>
+      </c>
+      <c r="F9">
+        <v>50</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>10981</v>
+      </c>
+      <c r="B10">
+        <v>9390</v>
+      </c>
+      <c r="C10">
+        <v>2621110</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>50</v>
+      </c>
+      <c r="F10">
+        <v>50</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10981</v>
+      </c>
+      <c r="B11">
+        <v>9391</v>
+      </c>
+      <c r="C11">
+        <v>2621111</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>50</v>
+      </c>
+      <c r="F11">
+        <v>50</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10981</v>
+      </c>
+      <c r="B12">
+        <v>9392</v>
+      </c>
+      <c r="C12">
+        <v>2621112</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>50</v>
+      </c>
+      <c r="F12">
+        <v>50</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>10981</v>
+      </c>
+      <c r="B13">
+        <v>9393</v>
+      </c>
+      <c r="C13">
+        <v>2621113</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>50</v>
+      </c>
+      <c r="F13">
+        <v>50</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>10981</v>
+      </c>
+      <c r="B14">
+        <v>9394</v>
+      </c>
+      <c r="C14">
+        <v>2621114</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="E14">
+        <v>50</v>
+      </c>
+      <c r="F14">
+        <v>50</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>10981</v>
+      </c>
+      <c r="B15">
+        <v>9395</v>
+      </c>
+      <c r="C15">
+        <v>2621115</v>
+      </c>
+      <c r="D15">
+        <v>3</v>
+      </c>
+      <c r="E15">
+        <v>50</v>
+      </c>
+      <c r="F15">
+        <v>50</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>10981</v>
+      </c>
+      <c r="B16">
+        <v>9396</v>
+      </c>
+      <c r="C16">
+        <v>2621116</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+      <c r="E16">
+        <v>50</v>
+      </c>
+      <c r="F16">
+        <v>50</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>

</xml_diff>

<commit_message>
- Added new package 0070-Misc-MAXDOMAIN: SKILLLEVEL, STE_CSWNEQPFUNCTN - Added new package 1005-Fix-DomainValue: JOBPLAN, JOBITEM - Added new package 1006-Fix-NI-Invoice
0017-Master-Companies:
- Copy custom columns from COMPMASTER

0063-Misc-JobPlan:
- Fixed: set JobPlan.CalcApplyTo="QUANTITY"

0065-Misc-JobMaterial
- Fixed: set JobItem.CalcApplyTo="QUANTITY"
- Fixed: set JobItem.CalcMethod="STATIC"

0307-PO-Invoice-InvoiceLine-InvoiceCost
- Fixed: set InvoiceLine.STE_MIGRATIONSOURCE, InvoiceCost.STE_MIGRATIONSOURCE
- Fixed: set Invoice.InvoiceNum for NI-Invoice = "NI-" + NI_REF
- Added: migrate NEG_INV_CC to InvoiceCost

0308-PO-MATRECTRANS-SERVRECTRANS
- Added: mapping to custom colums for RCT_ITEMS.RCT_QTY, RCT_ITEMS.RCT_VAL, RCT_ITEMS.ACP_QTY, RCT_ITEMS.RTN_TO_SUPL
</commit_message>
<xml_diff>
--- a/Integration Services Project2/notes/STR(DM-Transaction)-Appendix B - Test and PR Summary.xlsx
+++ b/Integration Services Project2/notes/STR(DM-Transaction)-Appendix B - Test and PR Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\STE.2022.CoswinMigration\Integration Services Project2\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B19F3B4D-3EB9-42E6-A13C-9A63871BE75C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AF94581-7B2A-4FC1-A4F7-190FD8A271A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="966" uniqueCount="469">
   <si>
     <t>Test Status</t>
   </si>
@@ -4004,6 +4004,95 @@
         <family val="3"/>
       </rPr>
       <t>(13,5)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> MAXIMO.MR </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF006464"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_CSWNDEMTYPE"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>INTEGER</t>
     </r>
     <r>
       <rPr>
@@ -12555,10 +12644,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB88DB5-3756-408C-974A-7C21E554649F}">
-  <dimension ref="A1:J139"/>
+  <dimension ref="A1:J141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="C132" sqref="C132"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="A135" sqref="A135:XFD136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -13573,22 +13662,22 @@
     </row>
     <row r="129" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B129" s="82" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
     </row>
     <row r="130" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B130" s="82" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
     </row>
     <row r="131" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B131" s="82" t="s">
-        <v>458</v>
+        <v>464</v>
       </c>
     </row>
     <row r="132" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B132" s="82" t="s">
-        <v>459</v>
+        <v>466</v>
       </c>
     </row>
     <row r="133" spans="2:2" x14ac:dyDescent="0.25">
@@ -13619,6 +13708,11 @@
     <row r="139" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B139" s="79" t="s">
         <v>463</v>
+      </c>
+    </row>
+    <row r="141" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B141" s="79" t="s">
+        <v>468</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Add new package 1006_Fix_Item_NONSTOCKFLAG: update the value of Item.STE_NONSTOCKFLAG column
0006-Master-Item:
- Added: new custom mapping STE_NONSTOCKFLAG (items from ITEM_ => 'N', items from NSITEM => 'Y')

0016-Master-CompMaster:
- Added: new custom mapping STE_CSWNSUPLTYPE (SUPPLIER_.S_SUPL_TYPE)

0017-Master-Companies:
- Added: new custom mapping STE_CSWNSUPLTYPE (SUPPLIER_.S_SUPL_TYPE)

0018-Master-Supplier-History:
- Fixed: hard-coded value for early0 (15), early1 (30), late0 (15), late1 (30), late2 (45), late3 (60)

0105-Asset-AssetTrans:
- Added: new mapping for sourcesysid (= EQP_MOVE.EM_ZONE)

0307-PO-Invoice-InvoiceLine-InvoiceCost
- Fixed: InvoiceCost is now in CostCenter level (mapped to Table INV_CC_INT instead of INV_ITEMS)
</commit_message>
<xml_diff>
--- a/Integration Services Project2/notes/STR(DM-Transaction)-Appendix B - Test and PR Summary.xlsx
+++ b/Integration Services Project2/notes/STR(DM-Transaction)-Appendix B - Test and PR Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\STE.2022.CoswinMigration\Integration Services Project2\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AF94581-7B2A-4FC1-A4F7-190FD8A271A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E83F0AA5-0E3E-4C45-B90A-76A08D846C17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="966" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="474">
   <si>
     <t>Test Status</t>
   </si>
@@ -4093,6 +4093,532 @@
         <family val="3"/>
       </rPr>
       <t>INTEGER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> MAXIMO.ITEM </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF006464"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_NONSTOCKFLAG"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>VARCHAR(1)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF956037"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO.COMPMASTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_CSWNSUPLTYPE"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>VARCHAR(1)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF956037"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO.COMPANIES</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_CSWNSUPLTYPE"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>VARCHAR(1)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF956037"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO.INVOICE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_CSWNSTRING3"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>VARCHAR(20)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF956037"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO.INVOICELINE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_CSWNITEMBASEVAL"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>DECIMAL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(18,2)</t>
     </r>
     <r>
       <rPr>
@@ -12644,10 +13170,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB88DB5-3756-408C-974A-7C21E554649F}">
-  <dimension ref="A1:J141"/>
+  <dimension ref="A1:J147"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="A135" sqref="A135:XFD136"/>
+      <selection activeCell="B145" sqref="B145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -13713,6 +14239,31 @@
     <row r="141" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B141" s="79" t="s">
         <v>468</v>
+      </c>
+    </row>
+    <row r="143" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B143" s="79" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="144" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B144" s="82" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="145" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B145" s="82" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="146" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B146" s="82" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="147" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B147" s="82" t="s">
+        <v>472</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
0401-WO-Workorder: - Fixed: missing lookup to asset location - Fixed: missing lookup to route location (using zone-to-location mapping)
0071-Misc-PersonCal:
- Fixed: only create calendar for active user
</commit_message>
<xml_diff>
--- a/Integration Services Project2/notes/STR(DM-Transaction)-Appendix B - Test and PR Summary.xlsx
+++ b/Integration Services Project2/notes/STR(DM-Transaction)-Appendix B - Test and PR Summary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\STE.2022.CoswinMigration\Integration Services Project2\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E83F0AA5-0E3E-4C45-B90A-76A08D846C17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4ADF9DE-901F-455A-816C-60732EC93FA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="978" uniqueCount="481">
   <si>
     <t>Test Status</t>
   </si>
@@ -4619,6 +4619,827 @@
         <family val="3"/>
       </rPr>
       <t>(18,2)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">.CALENDAR </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF006464"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONID"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>BIGINT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>CALENDAR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF006464"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONDATE"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TIMESTAMP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">.WORKPERIOD </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF006464"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONID"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>BIGINT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>WORKPERIOD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF006464"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONDATE"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TIMESTAMP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">.PERSONCAL </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF006464"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONID"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>BIGINT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>PERSONCAL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF006464"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONDATE"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TIMESTAMP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>INVOICE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF006464"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_CSWNISSUEDATE"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>DATE</t>
     </r>
     <r>
       <rPr>
@@ -13170,10 +13991,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB88DB5-3756-408C-974A-7C21E554649F}">
-  <dimension ref="A1:J147"/>
+  <dimension ref="A1:J157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="B145" sqref="B145"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="B157" sqref="B157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -14251,19 +15072,60 @@
         <v>473</v>
       </c>
     </row>
-    <row r="145" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B145" s="82" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="146" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B146" s="82" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="147" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B147" s="82" t="s">
         <v>472</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" s="73" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A149" s="72"/>
+      <c r="D149" s="74"/>
+      <c r="E149" s="74"/>
+      <c r="F149" s="74"/>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B151" s="79" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B152" s="79" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B153" s="79" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B154" s="79" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B155" s="79" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B156" s="79" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B157" s="79" t="s">
+        <v>480</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Load item master, location master and asset master from latest XLS - Migrate latest COSWIN backup (Feb 2025)
</commit_message>
<xml_diff>
--- a/Integration Services Project2/notes/STR(DM-Transaction)-Appendix B - Test and PR Summary.xlsx
+++ b/Integration Services Project2/notes/STR(DM-Transaction)-Appendix B - Test and PR Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\STE.2022.CoswinMigration\Integration Services Project2\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4ADF9DE-901F-455A-816C-60732EC93FA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B04DB83-9CE9-4BF6-9DE3-AF835C694A9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="978" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="981" uniqueCount="484">
   <si>
     <t>Test Status</t>
   </si>
@@ -5450,6 +5450,119 @@
       </rPr>
       <t>;</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">.PERSONGROUP </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF006464"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_DEPARTMENT"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>VARCHAR(16)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <t>RESIZE LOCATIONS.STE_TUNNEL TO 8 CHAR</t>
+  </si>
+  <si>
+    <t>RESIZE LOCATIONS.STE_TRAINAREA TO 4 CHAR</t>
   </si>
 </sst>
 </file>
@@ -5808,7 +5921,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -6038,6 +6151,13 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -13991,10 +14111,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB88DB5-3756-408C-974A-7C21E554649F}">
-  <dimension ref="A1:J157"/>
+  <dimension ref="A1:J160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="B157" sqref="B157"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="B160" sqref="B160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -15126,6 +15246,23 @@
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B157" s="79" t="s">
         <v>480</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B158" s="88" t="s">
+        <v>481</v>
+      </c>
+      <c r="C158" s="89"/>
+      <c r="D158" s="90"/>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B159" s="79" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B160" s="79" t="s">
+        <v>483</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
0101-Asset-Asset: - Fixed: Asset.ITEMNUM still using the coswin itemno instead of maximo itemnum
1104-File-Location:
- Added: filter against empty rows when loading XLSX
</commit_message>
<xml_diff>
--- a/Integration Services Project2/notes/STR(DM-Transaction)-Appendix B - Test and PR Summary.xlsx
+++ b/Integration Services Project2/notes/STR(DM-Transaction)-Appendix B - Test and PR Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\STE.2022.CoswinMigration\Integration Services Project2\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B04DB83-9CE9-4BF6-9DE3-AF835C694A9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CCC75BC-C82C-4F3E-834A-9713B62D371C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1776" yWindow="1776" windowWidth="17280" windowHeight="8880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Summary" sheetId="6" r:id="rId1"/>
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="981" uniqueCount="484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="488">
   <si>
     <t>Test Status</t>
   </si>
@@ -5452,6 +5452,12 @@
     </r>
   </si>
   <si>
+    <t>RESIZE LOCATIONS.STE_TUNNEL TO 8 CHAR</t>
+  </si>
+  <si>
+    <t>RESIZE LOCATIONS.STE_TRAINAREA TO 4 CHAR</t>
+  </si>
+  <si>
     <r>
       <t>ALTER</t>
     </r>
@@ -5499,7 +5505,7 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t xml:space="preserve">.PERSONGROUP </t>
+      <t xml:space="preserve">.STE_ITEM_MAINTENTITY </t>
     </r>
     <r>
       <rPr>
@@ -5527,7 +5533,7 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t>"STE_DEPARTMENT"</t>
+      <t>"STE_MIGRATIONID"</t>
     </r>
     <r>
       <rPr>
@@ -5546,6 +5552,238 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
+      <t>BIGINT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>STE_ITEM_MAINTENTITY</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF006464"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONDATE"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TIMESTAMP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">.ROUTES </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF006464"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_LOCTYPE"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
       <t>VARCHAR(16)</t>
     </r>
     <r>
@@ -5559,10 +5797,10 @@
     </r>
   </si>
   <si>
-    <t>RESIZE LOCATIONS.STE_TUNNEL TO 8 CHAR</t>
-  </si>
-  <si>
-    <t>RESIZE LOCATIONS.STE_TRAINAREA TO 4 CHAR</t>
+    <t>RESIZE LOCATIONS.STE_VIADUCT TO 8 CHAR.</t>
+  </si>
+  <si>
+    <t>RESIZE LOCATIONS.STE_TRACKNO TO 8 CHAR.</t>
   </si>
 </sst>
 </file>
@@ -5921,7 +6159,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -6151,13 +6389,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -14111,10 +14342,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB88DB5-3756-408C-974A-7C21E554649F}">
-  <dimension ref="A1:J160"/>
+  <dimension ref="A1:J167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="B160" sqref="B160"/>
+    <sheetView tabSelected="1" topLeftCell="A159" workbookViewId="0">
+      <selection activeCell="B167" sqref="B167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -15249,11 +15480,9 @@
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B158" s="88" t="s">
+      <c r="B158" s="79" t="s">
         <v>481</v>
       </c>
-      <c r="C158" s="89"/>
-      <c r="D158" s="90"/>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B159" s="79" t="s">
@@ -15263,6 +15492,32 @@
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B160" s="79" t="s">
         <v>483</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B161" s="79" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B162" s="79" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" s="73" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A164" s="72"/>
+      <c r="D164" s="74"/>
+      <c r="E164" s="74"/>
+      <c r="F164" s="74"/>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B166" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B167" t="s">
+        <v>487</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added: load asset-master-issues-(fixes).xlsx and update asset location/location type Fixed: Cannot schedule labor assignment for migrated user/labor Fixed: references to old WO causing WO creation error
0052-Master-Craft-CraftSkill:
- Set CraftSkill default to 'STANDARD'.
- Set CraftSkill.Description for STANDARD to Craft's description.

0055-Master-Labor-LaborCraftRate:
- Set Labor.AvailFactor=1
- Set default LaborCraftRate.skilllevel to 'STANDARD'

0056-Master-Crew
- Disable CREW migration for now because it makes it too complicated to schedule work

0058-Misc-PPCraftRate:
- Set default skilllevel to 'STANDARD'
- Only migrate premium rate when value>0

1010-Fix-Asset-Location:
- Added: load asset-master-issues-(fixes).xlsx and update asset location/location type

1019-Fix-Old-WO-References:
- Fixed: references to old WO causing WO creation error
</commit_message>
<xml_diff>
--- a/Integration Services Project2/notes/STR(DM-Transaction)-Appendix B - Test and PR Summary.xlsx
+++ b/Integration Services Project2/notes/STR(DM-Transaction)-Appendix B - Test and PR Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\STE.2022.CoswinMigration\Integration Services Project2\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CCC75BC-C82C-4F3E-834A-9713B62D371C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0F59792-38AB-4E2B-B31A-4F0B22948DD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1776" yWindow="1776" windowWidth="17280" windowHeight="8880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Summary" sheetId="6" r:id="rId1"/>
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="996" uniqueCount="499">
   <si>
     <t>Test Status</t>
   </si>
@@ -5801,6 +5801,1259 @@
   </si>
   <si>
     <t>RESIZE LOCATIONS.STE_TRACKNO TO 8 CHAR.</t>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF956037"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF8E00C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>PLUSTWOQUALFLG</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONID"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>BIGINT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF956037"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF8E00C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>PLUSTWOQUALFLG</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONDATE"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TIMESTAMP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF956037"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF8E00C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>WOANCESTOR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONID"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>BIGINT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>WOANCESTOR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF006464"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONDATE"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TIMESTAMP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>WOSERVICEADDRESS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF006464"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONID"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>BIGINT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>WOSERVICEADDRESS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF006464"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONDATE"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TIMESTAMP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>WOSTATUS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF006464"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONID"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>BIGINT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>WOSTATUS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF006464"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONDATE"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TIMESTAMP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>WORKVIEW</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF006464"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONID"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>BIGINT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>WORKVIEW</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF006464"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONDATE"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TIMESTAMP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <t>RESIZE LOCATIONS.STE_VIADUCTCOLUMNPIERCODE TO 8 CHAR.</t>
   </si>
 </sst>
 </file>
@@ -14342,10 +15595,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB88DB5-3756-408C-974A-7C21E554649F}">
-  <dimension ref="A1:J167"/>
+  <dimension ref="A1:J180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A159" workbookViewId="0">
-      <selection activeCell="B167" sqref="B167"/>
+    <sheetView tabSelected="1" topLeftCell="A156" workbookViewId="0">
+      <selection activeCell="A180" sqref="A180:XFD180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -15519,6 +16772,67 @@
       <c r="B167" t="s">
         <v>487</v>
       </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B168" s="79" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B169" s="79" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B170" s="79" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B171" s="79" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B172" s="79" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B173" s="79" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B174" s="79" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B175" s="79" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B176" s="79" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B177" s="79" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B178" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" s="73" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A180" s="72"/>
+      <c r="D180" s="74"/>
+      <c r="E180" s="74"/>
+      <c r="F180" s="74"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- Added: Load latest failure list file (XLSX) - Added: Load zone to location mapping - Added: Populate location related tables: LOCSTATUS, LOCOPER, LOCANCESTOR, LOCHIERARCHY - Fixed: Change location type RST to TRAIN
0003-Master-Locations:
- Fixed: to populate location components selectively based on location type

0014-Master-FailureCode-FailureList:
- Fixed: to load latest master file (xlsx)

0105-Asset-AssetTrans:
- Fixed: mapping fromparent and toparent
- Fixed: mapping fromloc and toloc using zone-to-location mapping

0114-Asset-RelatedTables:
- Fixed: to update JobPlan's system/subsyste/loctype from JPAssetsPLink and PM

1104-File-Location-Master:
- Fixed: to change location type from RST to TRAIN
</commit_message>
<xml_diff>
--- a/Integration Services Project2/notes/STR(DM-Transaction)-Appendix B - Test and PR Summary.xlsx
+++ b/Integration Services Project2/notes/STR(DM-Transaction)-Appendix B - Test and PR Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\STE.2022.CoswinMigration\Integration Services Project2\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FD43578-A601-4406-A595-221A683EC3EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8325E362-B4D3-4026-B6F4-CD82CBBF8D4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1006" uniqueCount="509">
   <si>
     <t>Test Status</t>
   </si>
@@ -7488,6 +7488,702 @@
         <family val="3"/>
       </rPr>
       <t>LOCHIERARCHY</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONDATE"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TIMESTAMP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF956037"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">.LABORSTATUS </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONID"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>BIGINT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF956037"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF8E00C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>LABORSTATUS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONDATE"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TIMESTAMP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF956037"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">.LOCOPER </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONID"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>BIGINT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF956037"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF8E00C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>LOCOPER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONDATE"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TIMESTAMP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF956037"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">.LOCSTATUS </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONID"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>BIGINT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF956037"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF8E00C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>LOCSTATUS</t>
     </r>
     <r>
       <rPr>
@@ -16095,10 +16791,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB88DB5-3756-408C-974A-7C21E554649F}">
-  <dimension ref="A1:J185"/>
+  <dimension ref="A1:J191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A162" workbookViewId="0">
-      <selection activeCell="B185" activeCellId="1" sqref="B184 B185"/>
+    <sheetView tabSelected="1" topLeftCell="A168" workbookViewId="0">
+      <selection activeCell="B190" sqref="B190:B191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -17352,6 +18048,36 @@
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B185" s="79" t="s">
         <v>502</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B186" s="79" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B187" s="79" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B188" s="79" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B189" s="79" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B190" s="79" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B191" s="79" t="s">
+        <v>508</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Move updating Route/PM/JobPlan system/subsystem/loctype to 0101-Asset-Asset - Fixed: duplicate failure report for given WO is to be stored in custom table STE_ALTFAILURECODE
0011-Master-Routes:
- Added: populate STE_CSWNAUTHORITY from EQP_TOPO.EQ_EQAUTHORITY

0101-Asset-Asset:
- Added: update Route/PM/JobPlan system/subsystem/loctype from Asset

0401-W0-Workorder:
- Fixed: to set WO's STE_LINE/STE_SYSTEM/STE_SUBSYSTEM/CSWNEQAUTHORITY from
Asset/Route
- Fixed: to set WO.STE_MAINTENTITY based on CSWNACTIONAUTH/CSWNEQAUTHORITY

0406-WO-FailureReport:
- Added: populate STE_ALTFAILURECODE
- Fixed: duplicate failure report for given WO is to be stored in custom table STE_ALTFAILURECODE
- Fixed: only migrate to FailureReport/STE_ALTFAILURECODE those records with valid WO reference

0713-Others-TransactionTable8
- Added: migrate EQP_DEFR as-is since only records with valid WO reference are migrated to FailureReport/STE_ALTFAILURECODE
</commit_message>
<xml_diff>
--- a/Integration Services Project2/notes/STR(DM-Transaction)-Appendix B - Test and PR Summary.xlsx
+++ b/Integration Services Project2/notes/STR(DM-Transaction)-Appendix B - Test and PR Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\STE.2022.CoswinMigration\Integration Services Project2\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8325E362-B4D3-4026-B6F4-CD82CBBF8D4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B78D7E-4EEC-4D35-ABF3-7A9E2F39D1FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1006" uniqueCount="509">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="514">
   <si>
     <t>Test Status</t>
   </si>
@@ -8184,6 +8184,649 @@
         <family val="3"/>
       </rPr>
       <t>LOCSTATUS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONDATE"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TIMESTAMP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF956037"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF8E00C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>LABTRANS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF006464"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONWOREF"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>BIGINT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF956037"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF8E00C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ROUTES</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_CSWNAUTHORITY"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>VARCHAR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>16</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF956037"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">.WORKORDER </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_CSWNEQAUTHORITY"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>VARCHAR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>16</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF956037"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">.STE_ALTFAILURECODE </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONID"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>BIGINT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF956037"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF8E00C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>STE_ALTFAILURECODE</t>
     </r>
     <r>
       <rPr>
@@ -16791,10 +17434,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB88DB5-3756-408C-974A-7C21E554649F}">
-  <dimension ref="A1:J191"/>
+  <dimension ref="A1:J199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A168" workbookViewId="0">
-      <selection activeCell="B190" sqref="B190:B191"/>
+    <sheetView tabSelected="1" topLeftCell="A174" workbookViewId="0">
+      <selection activeCell="A194" sqref="A194:XFD194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -18078,6 +18721,37 @@
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B191" s="79" t="s">
         <v>508</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B192" s="82" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" s="73" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A194" s="72"/>
+      <c r="D194" s="74"/>
+      <c r="E194" s="74"/>
+      <c r="F194" s="74"/>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B196" s="82" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B197" s="82" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B198" s="79" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B199" s="79" t="s">
+        <v>513</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Added 1042-Fix-ALNDOMAIN-SiteId-OrgId: To reset ALNDOMAIN.ORGID and SITEID to NULL for all additional MAXDOMAIN - Added 1043-Fix-WorkType-Type: to set WORKTYPE.TYPE to 'NONE' for migrated data - Added 1044-Fix-Asset-STE-CDTYPE: to set Asset.STE_CDTYPE='CD' for all Assets which has description ends with '(CD)'
0062-Misc-WorkType:
- Fixed: to set WORKTYPE.TYPE to 'NONE' for migrated data

0070-Misc-MAXDOMAIN:
- Fixed: to set ALNDOMAIN.ORGID and SITEID to NULL for all additional MAXDOMAIN

0101-Asset-Asset:
- Fixed: to set Asset.STE_CDTYPE='CD' for all Assets which has description ends with '(CD)'
</commit_message>
<xml_diff>
--- a/Integration Services Project2/notes/STR(DM-Transaction)-Appendix B - Test and PR Summary.xlsx
+++ b/Integration Services Project2/notes/STR(DM-Transaction)-Appendix B - Test and PR Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\STE.2022.CoswinMigration\Integration Services Project2\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3498454A-6009-49A2-9E10-F7A91A22F2C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E8F30B-A5E4-4F29-ACA5-433EEDB380A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="528">
   <si>
     <t>Test Status</t>
   </si>
@@ -9895,6 +9895,292 @@
         <family val="3"/>
       </rPr>
       <t>TIMESTAMP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF956037"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF8E00C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>INVUSE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF006464"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_CSWNDEMREF"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>VARCHAR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF956037"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF8E00C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>INVUSE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_CSWNORIGDEMREF"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>VARCHAR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(8)</t>
     </r>
     <r>
       <rPr>
@@ -18446,10 +18732,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB88DB5-3756-408C-974A-7C21E554649F}">
-  <dimension ref="A1:J209"/>
+  <dimension ref="A1:J213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A189" workbookViewId="0">
-      <selection activeCell="B204" sqref="B204:B209"/>
+    <sheetView tabSelected="1" topLeftCell="A192" workbookViewId="0">
+      <selection activeCell="A213" sqref="A213:XFD213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -19814,10 +20100,26 @@
         <v>524</v>
       </c>
     </row>
-    <row r="209" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B209" s="79" t="s">
         <v>525</v>
       </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B210" s="79" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B211" s="79" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" s="73" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A213" s="72"/>
+      <c r="D213" s="74"/>
+      <c r="E213" s="74"/>
+      <c r="F213" s="74"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- Added: 0023-Master-ItemStatus-ItemOrgStatus - Added: 0212-Inventory-MRCost-MRStatus - Added: 0213-Inventory-InvUseLineSplit-InvUseStatus - Fixed: InvReserve.ActualQuantity => issued qty so far for the given reservation
0211-Inventory-InvReserve-Mr:
- Fixed: InvReserve.ActualQuantity => issued qty so far for the given reservation
</commit_message>
<xml_diff>
--- a/Integration Services Project2/notes/STR(DM-Transaction)-Appendix B - Test and PR Summary.xlsx
+++ b/Integration Services Project2/notes/STR(DM-Transaction)-Appendix B - Test and PR Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\STE.2022.CoswinMigration\Integration Services Project2\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:2001_{60598C80-8C4F-4EF5-BCD1-F84F230A08CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BEAAF89-4813-477E-98B3-378EF3888C19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,6 @@
     <definedName name="TestVer">#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -97,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="555">
   <si>
     <t>Test Status</t>
   </si>
@@ -11456,6 +11455,1836 @@
         <family val="3"/>
       </rPr>
       <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">.ITEM </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF006464"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_CSWNITEMCC"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>VARCHAR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF956037"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">.MRSTATUS </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONID"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>BIGINT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF956037"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF8E00C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MRSTATUS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONDATE"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TIMESTAMP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF956037"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">.INVSTATUS </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONID"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>BIGINT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF956037"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF8E00C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>INVSTATUS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONDATE"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TIMESTAMP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF956037"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">.MRCOST </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONID"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>BIGINT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF956037"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF8E00C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MRCOST</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONDATE"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TIMESTAMP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF956037"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF8E00C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ITEMSTATUS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONID"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>BIGINT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF956037"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF8E00C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ITEMSTATUS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONDATE"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TIMESTAMP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF956037"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF8E00C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ITEMORGSTATUS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONID"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>BIGINT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF956037"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF8E00C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ITEMORGSTATUS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONDATE"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TIMESTAMP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF956037"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF8E00C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>INVUSELINESPLIT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONID"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>BIGINT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF956037"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF8E00C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>INVUSELINESPLIT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONDATE"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TIMESTAMP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF956037"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF8E00C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>INVUSESTATUS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONID"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>BIGINT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF956037"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF8E00C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>INVUSESTATUS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONDATE"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TIMESTAMP</t>
     </r>
     <r>
       <rPr>
@@ -11824,7 +13653,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -12055,10 +13884,8 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -20012,10 +21839,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB88DB5-3756-408C-974A-7C21E554649F}">
-  <dimension ref="A1:J229"/>
+  <dimension ref="A1:J250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A174" workbookViewId="0">
-      <selection activeCell="B224" sqref="B224:B229"/>
+    <sheetView tabSelected="1" topLeftCell="A231" workbookViewId="0">
+      <selection activeCell="B246" sqref="B246"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -21431,40 +23258,134 @@
         <v>533</v>
       </c>
     </row>
-    <row r="222" spans="1:6" s="89" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A222" s="88"/>
-      <c r="D222" s="90"/>
-      <c r="E222" s="90"/>
-      <c r="F222" s="90"/>
+    <row r="222" spans="1:6" s="73" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A222" s="72"/>
+      <c r="D222" s="74"/>
+      <c r="E222" s="74"/>
+      <c r="F222" s="74"/>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B224" t="s">
         <v>534</v>
       </c>
     </row>
-    <row r="225" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B225" s="82" t="s">
         <v>535</v>
       </c>
     </row>
-    <row r="226" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B226" s="79" t="s">
         <v>537</v>
       </c>
     </row>
-    <row r="227" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B227" s="79" t="s">
         <v>538</v>
       </c>
     </row>
-    <row r="228" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B228" s="79" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="229" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B229" s="79" t="s">
         <v>539</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" s="73" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A231" s="72"/>
+      <c r="D231" s="74"/>
+      <c r="E231" s="74"/>
+      <c r="F231" s="74"/>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B233" s="79" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B234" s="79" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B235" s="79" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B236" s="79" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B237" s="79" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B238" s="79"/>
+    </row>
+    <row r="239" spans="1:6" s="73" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A239" s="72"/>
+      <c r="B239" s="88"/>
+      <c r="D239" s="74"/>
+      <c r="E239" s="74"/>
+      <c r="F239" s="74"/>
+    </row>
+    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B240" s="79"/>
+    </row>
+    <row r="241" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B241" s="79" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="242" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B242" s="79" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="243" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B243" s="79" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="244" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B244" s="79" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="245" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B245" s="79" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="246" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B246" s="79" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="247" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B247" s="79" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="248" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B248" s="79" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="249" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B249" s="79" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="250" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B250" s="79" t="s">
+        <v>554</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Added 1072-Fix-Item-GLAccount: to park Asset/Inventory/InvCost/InvTrans under cost centre '0000000' if cost centre value from coswin is not active (start with '2x'). Coswin value is stored in custom column. Note: There is already a logic to do cost centre replacement. But the mapping is not yet provided by SBST.
0101-Asset-Asset:
- Fixed: to park Asset/Inventory/InvCost/InvTrans under cost centre '0000000' if cost centre value from coswin is not active (start with '2x').

0201-Inventory-Inventory
- Fixed: to park Asset/Inventory/InvCost/InvTrans under cost centre '0000000' if cost centre value from coswin is not active (start with '2x').

0204-Inventory-InvCost
- Fixed: to park Asset/Inventory/InvCost/InvTrans under cost centre '0000000' if cost centre value from coswin is not active (start with '2x').

0206-Inventory-InvTrans:
- Fixed: to park Asset/Inventory/InvCost/InvTrans under cost centre '0000000' if cost centre value from coswin is not active (start with '2x').
</commit_message>
<xml_diff>
--- a/Integration Services Project2/notes/STR(DM-Transaction)-Appendix B - Test and PR Summary.xlsx
+++ b/Integration Services Project2/notes/STR(DM-Transaction)-Appendix B - Test and PR Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\STE.2022.CoswinMigration\Integration Services Project2\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E997F1-9008-4081-8C13-5569EF098DFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{541C4562-2917-4CDE-BA36-85456B595DFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="557">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1058" uniqueCount="561">
   <si>
     <t>Test Status</t>
   </si>
@@ -13413,6 +13413,515 @@
         <family val="3"/>
       </rPr>
       <t>VARCHAR(16)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF956037"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">.TICKET </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_COSWINCC"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>VARCHAR(16)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">.INVENTORY </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF006464"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_COSWINCC"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>VARCHAR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">.ASSET </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF006464"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_CSWNEQCOSC"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>VARCHAR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">.ROUTES </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF006464"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_CSWNEQCOSC"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>VARCHAR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
     </r>
     <r>
       <rPr>
@@ -13997,6 +14506,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -14011,9 +14523,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -14965,18 +15474,18 @@
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="C3" s="83" t="s">
+      <c r="C3" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="83"/>
-      <c r="E3" s="83"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="85" t="s">
+      <c r="D3" s="84"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="86" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="86"/>
-      <c r="I3" s="86"/>
-      <c r="J3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="88"/>
       <c r="K3" s="3" t="s">
         <v>61</v>
       </c>
@@ -21967,10 +22476,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB88DB5-3756-408C-974A-7C21E554649F}">
-  <dimension ref="A1:J252"/>
+  <dimension ref="A1:J256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A213" workbookViewId="0">
-      <selection activeCell="B252" sqref="B252"/>
+    <sheetView tabSelected="1" topLeftCell="A240" workbookViewId="0">
+      <selection activeCell="C245" sqref="C245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -23458,7 +23967,7 @@
     </row>
     <row r="239" spans="1:6" s="73" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A239" s="72"/>
-      <c r="B239" s="88"/>
+      <c r="B239" s="83"/>
       <c r="D239" s="74"/>
       <c r="E239" s="74"/>
       <c r="F239" s="74"/>
@@ -23524,6 +24033,26 @@
     <row r="252" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B252" s="79" t="s">
         <v>556</v>
+      </c>
+    </row>
+    <row r="253" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B253" s="79" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="254" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B254" s="79" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="255" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B255" s="79" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="256" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B256" s="79" t="s">
+        <v>560</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Add: 1227_Fix_Item_Catalog_Blob: load blob data for images for item image catalog - Add: 1228_Fix_Item_Catalog_FileSize: load image filesize to filter duplicate when creating item attachment entries
</commit_message>
<xml_diff>
--- a/Integration Services Project2/notes/STR(DM-Transaction)-Appendix B - Test and PR Summary.xlsx
+++ b/Integration Services Project2/notes/STR(DM-Transaction)-Appendix B - Test and PR Summary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\STE.2022.CoswinMigration\Integration Services Project2\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A36DEB8E-CE7F-469F-8A5C-04FA553FF8D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB540B0-27D7-4DD3-8FBE-E0F2A8EED95B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1059" uniqueCount="562">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1065" uniqueCount="568">
   <si>
     <t>Test Status</t>
   </si>
@@ -14056,6 +14056,702 @@
         <family val="3"/>
       </rPr>
       <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF956037"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">.DOCINFO </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONID"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>BIGINT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF956037"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF8E00C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>DOCINFO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONDATE"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TIMESTAMP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF956037"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">.DOCLINKS </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONID"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>BIGINT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF956037"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF8E00C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>DOCLINKS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONDATE"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TIMESTAMP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF956037"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">.IMGLIB </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONID"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>BIGINT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF956037"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MAXIMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF8E00C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>IMGLIB</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6C5151"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"STE_MIGRATIONDATE"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TIMESTAMP</t>
     </r>
     <r>
       <rPr>
@@ -22610,10 +23306,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB88DB5-3756-408C-974A-7C21E554649F}">
-  <dimension ref="A1:J260"/>
+  <dimension ref="A1:J269"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A237" workbookViewId="0">
-      <selection activeCell="A258" sqref="A258:XFD258"/>
+    <sheetView tabSelected="1" topLeftCell="A244" workbookViewId="0">
+      <selection activeCell="B270" sqref="B270"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -24198,6 +24894,42 @@
     <row r="260" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B260" s="79" t="s">
         <v>561</v>
+      </c>
+    </row>
+    <row r="262" spans="1:6" s="73" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A262" s="72"/>
+      <c r="D262" s="74"/>
+      <c r="E262" s="74"/>
+      <c r="F262" s="74"/>
+    </row>
+    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B264" s="79" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B265" s="79" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B266" s="79" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B267" s="79" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B268" s="79" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B269" s="79" t="s">
+        <v>567</v>
       </c>
     </row>
   </sheetData>

</xml_diff>